<commit_message>
Update after feedback from K.H
</commit_message>
<xml_diff>
--- a/output/grimm_measures.xlsx
+++ b/output/grimm_measures.xlsx
@@ -1730,13 +1730,13 @@
         <v>82.1675</v>
       </c>
       <c r="M2" t="n">
-        <v>5.85282208588957</v>
+        <v>0.588743073047858</v>
       </c>
       <c r="N2" t="n">
-        <v>4.10231083844581</v>
+        <v>0.422508816120907</v>
       </c>
       <c r="O2" t="n">
-        <v>5.55192229038855</v>
+        <v>0.471841309823678</v>
       </c>
     </row>
     <row r="3">
@@ -1777,13 +1777,13 @@
         <v>94.5850902344409</v>
       </c>
       <c r="M3" t="n">
-        <v>5.84642324888226</v>
+        <v>0.600565789473684</v>
       </c>
       <c r="N3" t="n">
-        <v>4.21934426229508</v>
+        <v>0.435406015037594</v>
       </c>
       <c r="O3" t="n">
-        <v>5.57757078986587</v>
+        <v>0.495966165413534</v>
       </c>
     </row>
     <row r="4">
@@ -1824,13 +1824,13 @@
         <v>50.9973333333333</v>
       </c>
       <c r="M4" t="n">
-        <v>5.66829704510109</v>
+        <v>0.5637097107438</v>
       </c>
       <c r="N4" t="n">
-        <v>4.11402799377916</v>
+        <v>0.461081611570248</v>
       </c>
       <c r="O4" t="n">
-        <v>5.53171073094868</v>
+        <v>0.503064049586778</v>
       </c>
     </row>
     <row r="5">
@@ -1871,13 +1871,13 @@
         <v>66.7566568047337</v>
       </c>
       <c r="M5" t="n">
-        <v>5.79746268656716</v>
+        <v>0.576943037974683</v>
       </c>
       <c r="N5" t="n">
-        <v>4.14656716417911</v>
+        <v>0.433996835443038</v>
       </c>
       <c r="O5" t="n">
-        <v>5.53333333333333</v>
+        <v>0.474386075949367</v>
       </c>
     </row>
     <row r="6">
@@ -1918,13 +1918,13 @@
         <v>91.2890625</v>
       </c>
       <c r="M6" t="n">
-        <v>5.85605975723623</v>
+        <v>0.619119503945886</v>
       </c>
       <c r="N6" t="n">
-        <v>4.17616246498599</v>
+        <v>0.461418263810599</v>
       </c>
       <c r="O6" t="n">
-        <v>5.676918767507</v>
+        <v>0.543047350620068</v>
       </c>
     </row>
     <row r="7">
@@ -1959,19 +1959,19 @@
         <v>0.419087136929461</v>
       </c>
       <c r="K7" t="n">
-        <v>0.580912863070539</v>
+        <v>0.58091286307054</v>
       </c>
       <c r="L7" t="n">
         <v>67.0979822906082</v>
       </c>
       <c r="M7" t="n">
-        <v>5.81646728971963</v>
+        <v>0.605807785888078</v>
       </c>
       <c r="N7" t="n">
-        <v>4.21977570093458</v>
+        <v>0.457591240875913</v>
       </c>
       <c r="O7" t="n">
-        <v>5.69530841121495</v>
+        <v>0.542481751824818</v>
       </c>
     </row>
     <row r="8">
@@ -2012,13 +2012,13 @@
         <v>86.5033910034602</v>
       </c>
       <c r="M8" t="n">
-        <v>5.89135401974612</v>
+        <v>0.624484674329502</v>
       </c>
       <c r="N8" t="n">
-        <v>4.18445698166432</v>
+        <v>0.435086206896551</v>
       </c>
       <c r="O8" t="n">
-        <v>5.6240197461213</v>
+        <v>0.516749042145594</v>
       </c>
     </row>
     <row r="9">
@@ -2059,13 +2059,13 @@
         <v>55.9609375</v>
       </c>
       <c r="M9" t="n">
-        <v>5.83928653624856</v>
+        <v>0.599230769230768</v>
       </c>
       <c r="N9" t="n">
-        <v>4.15210586881473</v>
+        <v>0.430568940493469</v>
       </c>
       <c r="O9" t="n">
-        <v>5.60493670886076</v>
+        <v>0.492349782293179</v>
       </c>
     </row>
     <row r="10">
@@ -2106,13 +2106,13 @@
         <v>84.7728928199792</v>
       </c>
       <c r="M10" t="n">
-        <v>5.82538461538462</v>
+        <v>0.580500000000001</v>
       </c>
       <c r="N10" t="n">
-        <v>4.09636752136752</v>
+        <v>0.446932065217392</v>
       </c>
       <c r="O10" t="n">
-        <v>5.55621794871795</v>
+        <v>0.480342391304348</v>
       </c>
     </row>
     <row r="11">
@@ -2153,13 +2153,13 @@
         <v>74.8515165233137</v>
       </c>
       <c r="M11" t="n">
-        <v>5.91315245478036</v>
+        <v>0.608999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>4.13332041343669</v>
+        <v>0.411394557823129</v>
       </c>
       <c r="O11" t="n">
-        <v>5.6397157622739</v>
+        <v>0.476360544217687</v>
       </c>
     </row>
     <row r="12">
@@ -2200,13 +2200,13 @@
         <v>86.870479947403</v>
       </c>
       <c r="M12" t="n">
-        <v>5.81551948051948</v>
+        <v>0.601991379310345</v>
       </c>
       <c r="N12" t="n">
-        <v>4.06857142857143</v>
+        <v>0.452935344827586</v>
       </c>
       <c r="O12" t="n">
-        <v>5.64191558441558</v>
+        <v>0.48848275862069</v>
       </c>
     </row>
     <row r="13">
@@ -2247,13 +2247,13 @@
         <v>62.1511111111111</v>
       </c>
       <c r="M13" t="n">
-        <v>5.79244821092279</v>
+        <v>0.568966501240695</v>
       </c>
       <c r="N13" t="n">
-        <v>4.05662900188324</v>
+        <v>0.393272952853597</v>
       </c>
       <c r="O13" t="n">
-        <v>5.60587570621469</v>
+        <v>0.448790322580644</v>
       </c>
     </row>
     <row r="14">
@@ -2294,13 +2294,13 @@
         <v>98.9839476813317</v>
       </c>
       <c r="M14" t="n">
-        <v>5.56614785992218</v>
+        <v>0.569544303797468</v>
       </c>
       <c r="N14" t="n">
-        <v>4.27009727626459</v>
+        <v>0.482053164556962</v>
       </c>
       <c r="O14" t="n">
-        <v>5.45066147859922</v>
+        <v>0.539936708860759</v>
       </c>
     </row>
     <row r="15">
@@ -2341,13 +2341,13 @@
         <v>128.692520775623</v>
       </c>
       <c r="M15" t="n">
-        <v>5.78698996655518</v>
+        <v>0.596045652173913</v>
       </c>
       <c r="N15" t="n">
-        <v>4.12295986622074</v>
+        <v>0.438828260869565</v>
       </c>
       <c r="O15" t="n">
-        <v>5.55070234113712</v>
+        <v>0.505678260869565</v>
       </c>
     </row>
     <row r="16">
@@ -2388,13 +2388,13 @@
         <v>75.0524099820183</v>
       </c>
       <c r="M16" t="n">
-        <v>5.7200819000819</v>
+        <v>0.577877766069545</v>
       </c>
       <c r="N16" t="n">
-        <v>4.11230139230139</v>
+        <v>0.419068493150686</v>
       </c>
       <c r="O16" t="n">
-        <v>5.66561015561016</v>
+        <v>0.498259220231822</v>
       </c>
     </row>
     <row r="17">
@@ -2435,13 +2435,13 @@
         <v>88.1263696128561</v>
       </c>
       <c r="M17" t="n">
-        <v>5.93915577889447</v>
+        <v>0.597679841897231</v>
       </c>
       <c r="N17" t="n">
-        <v>4.02456281407035</v>
+        <v>0.406836627140975</v>
       </c>
       <c r="O17" t="n">
-        <v>5.6029648241206</v>
+        <v>0.464947299077734</v>
       </c>
     </row>
     <row r="18">
@@ -2482,13 +2482,13 @@
         <v>65.6917360285374</v>
       </c>
       <c r="M18" t="n">
-        <v>5.65542168674699</v>
+        <v>0.56891935483871</v>
       </c>
       <c r="N18" t="n">
-        <v>4.16344578313253</v>
+        <v>0.43991935483871</v>
       </c>
       <c r="O18" t="n">
-        <v>5.47698795180723</v>
+        <v>0.491561290322581</v>
       </c>
     </row>
     <row r="19">
@@ -2529,13 +2529,13 @@
         <v>39.0542315631451</v>
       </c>
       <c r="M19" t="n">
-        <v>5.76670984455959</v>
+        <v>0.576416666666667</v>
       </c>
       <c r="N19" t="n">
-        <v>4.1199481865285</v>
+        <v>0.423910256410256</v>
       </c>
       <c r="O19" t="n">
-        <v>5.55774611398964</v>
+        <v>0.474580128205128</v>
       </c>
     </row>
     <row r="20">
@@ -2576,13 +2576,13 @@
         <v>84.371875</v>
       </c>
       <c r="M20" t="n">
-        <v>5.88864306784661</v>
+        <v>0.583161825726141</v>
       </c>
       <c r="N20" t="n">
-        <v>4.12587020648968</v>
+        <v>0.407062240663901</v>
       </c>
       <c r="O20" t="n">
-        <v>5.56598820058997</v>
+        <v>0.467319502074689</v>
       </c>
     </row>
     <row r="21">
@@ -2611,7 +2611,7 @@
         <v>0.657692307692308</v>
       </c>
       <c r="I21" t="n">
-        <v>50.8241758241758</v>
+        <v>50.958904109589</v>
       </c>
       <c r="J21" t="n">
         <v>0.489767113620325</v>
@@ -2623,13 +2623,13 @@
         <v>54.216932132964</v>
       </c>
       <c r="M21" t="n">
-        <v>5.91584870848708</v>
+        <v>0.586405829596412</v>
       </c>
       <c r="N21" t="n">
-        <v>4.09983394833948</v>
+        <v>0.385363228699552</v>
       </c>
       <c r="O21" t="n">
-        <v>5.61931734317343</v>
+        <v>0.447710762331839</v>
       </c>
     </row>
     <row r="22">
@@ -2670,13 +2670,13 @@
         <v>104.808673469388</v>
       </c>
       <c r="M22" t="n">
-        <v>5.68634228187919</v>
+        <v>0.568690677966102</v>
       </c>
       <c r="N22" t="n">
-        <v>4.18751677852349</v>
+        <v>0.454266949152542</v>
       </c>
       <c r="O22" t="n">
-        <v>5.45748322147651</v>
+        <v>0.518487288135593</v>
       </c>
     </row>
     <row r="23">
@@ -2717,13 +2717,13 @@
         <v>73.79168</v>
       </c>
       <c r="M23" t="n">
-        <v>5.8797320471597</v>
+        <v>0.604938235294116</v>
       </c>
       <c r="N23" t="n">
-        <v>4.10060021436227</v>
+        <v>0.441486764705881</v>
       </c>
       <c r="O23" t="n">
-        <v>5.59809217577706</v>
+        <v>0.510163235294118</v>
       </c>
     </row>
     <row r="24">
@@ -2755,22 +2755,22 @@
         <v>46.0215053763441</v>
       </c>
       <c r="J24" t="n">
-        <v>0.449529512403764</v>
+        <v>0.449957228400342</v>
       </c>
       <c r="K24" t="n">
-        <v>0.550470487596236</v>
+        <v>0.550042771599658</v>
       </c>
       <c r="L24" t="n">
         <v>95.6669146561803</v>
       </c>
       <c r="M24" t="n">
-        <v>5.91575147928994</v>
+        <v>0.614094801223241</v>
       </c>
       <c r="N24" t="n">
-        <v>4.08951479289941</v>
+        <v>0.42380122324159</v>
       </c>
       <c r="O24" t="n">
-        <v>5.63609467455621</v>
+        <v>0.507266055045872</v>
       </c>
     </row>
     <row r="25">
@@ -2811,13 +2811,13 @@
         <v>5.40571088637716</v>
       </c>
       <c r="M25" t="n">
-        <v>6.21501694915254</v>
+        <v>0.638641304347827</v>
       </c>
       <c r="N25" t="n">
-        <v>4.08308474576271</v>
+        <v>0.376815217391305</v>
       </c>
       <c r="O25" t="n">
-        <v>5.7208813559322</v>
+        <v>0.466257246376812</v>
       </c>
     </row>
     <row r="26">
@@ -2858,13 +2858,13 @@
         <v>97.5103878116343</v>
       </c>
       <c r="M26" t="n">
-        <v>5.77735294117647</v>
+        <v>0.588565789473684</v>
       </c>
       <c r="N26" t="n">
-        <v>4.08294117647059</v>
+        <v>0.434802631578948</v>
       </c>
       <c r="O26" t="n">
-        <v>5.57820261437909</v>
+        <v>0.545429824561404</v>
       </c>
     </row>
     <row r="27">
@@ -2896,22 +2896,22 @@
         <v>43.448275862069</v>
       </c>
       <c r="J27" t="n">
-        <v>0.451301115241636</v>
+        <v>0.450557620817844</v>
       </c>
       <c r="K27" t="n">
-        <v>0.548698884758364</v>
+        <v>0.549442379182156</v>
       </c>
       <c r="L27" t="n">
         <v>90.3654931470035</v>
       </c>
       <c r="M27" t="n">
-        <v>5.64979357798165</v>
+        <v>0.568020467836258</v>
       </c>
       <c r="N27" t="n">
-        <v>4.07275229357798</v>
+        <v>0.429394736842106</v>
       </c>
       <c r="O27" t="n">
-        <v>5.59128440366973</v>
+        <v>0.485932748538012</v>
       </c>
     </row>
     <row r="28">
@@ -2949,16 +2949,16 @@
         <v>0.534307331072267</v>
       </c>
       <c r="L28" t="n">
-        <v>62.1605320699708</v>
+        <v>59.698975</v>
       </c>
       <c r="M28" t="n">
-        <v>5.77950653120464</v>
+        <v>0.583379472693032</v>
       </c>
       <c r="N28" t="n">
-        <v>4.07108127721335</v>
+        <v>0.413863465160077</v>
       </c>
       <c r="O28" t="n">
-        <v>5.60774310595065</v>
+        <v>0.478442561205274</v>
       </c>
     </row>
     <row r="29">
@@ -2999,13 +2999,13 @@
         <v>63.3024503919215</v>
       </c>
       <c r="M29" t="n">
-        <v>5.78520053475936</v>
+        <v>0.581271944922547</v>
       </c>
       <c r="N29" t="n">
-        <v>4.09933155080214</v>
+        <v>0.428127366609294</v>
       </c>
       <c r="O29" t="n">
-        <v>5.56645721925134</v>
+        <v>0.487048192771084</v>
       </c>
     </row>
     <row r="30">
@@ -3046,13 +3046,13 @@
         <v>100.1325</v>
       </c>
       <c r="M30" t="n">
-        <v>5.95304812834225</v>
+        <v>0.643659259259259</v>
       </c>
       <c r="N30" t="n">
-        <v>4.11828877005348</v>
+        <v>0.388192592592592</v>
       </c>
       <c r="O30" t="n">
-        <v>5.69122994652406</v>
+        <v>0.495688888888889</v>
       </c>
     </row>
     <row r="31">
@@ -3093,13 +3093,13 @@
         <v>71.6803296948095</v>
       </c>
       <c r="M31" t="n">
-        <v>5.76016427104723</v>
+        <v>0.584564738292011</v>
       </c>
       <c r="N31" t="n">
-        <v>4.13813141683778</v>
+        <v>0.439162534435261</v>
       </c>
       <c r="O31" t="n">
-        <v>5.54535934291581</v>
+        <v>0.486118457300275</v>
       </c>
     </row>
     <row r="32">
@@ -3140,13 +3140,13 @@
         <v>50.8571428571429</v>
       </c>
       <c r="M32" t="n">
-        <v>5.62274261603376</v>
+        <v>0.545264044943821</v>
       </c>
       <c r="N32" t="n">
-        <v>4.05548523206751</v>
+        <v>0.436926966292134</v>
       </c>
       <c r="O32" t="n">
-        <v>5.5131223628692</v>
+        <v>0.468584269662921</v>
       </c>
     </row>
     <row r="33">
@@ -3187,13 +3187,13 @@
         <v>26.8305785123967</v>
       </c>
       <c r="M33" t="n">
-        <v>5.6052688172043</v>
+        <v>0.492538461538462</v>
       </c>
       <c r="N33" t="n">
-        <v>4.23784946236559</v>
+        <v>0.455569230769231</v>
       </c>
       <c r="O33" t="n">
-        <v>5.50709677419355</v>
+        <v>0.493723076923077</v>
       </c>
     </row>
     <row r="34">
@@ -3234,13 +3234,13 @@
         <v>82.9615912208505</v>
       </c>
       <c r="M34" t="n">
-        <v>5.64122494432071</v>
+        <v>0.56537570621469</v>
       </c>
       <c r="N34" t="n">
-        <v>4.2032293986637</v>
+        <v>0.468646892655368</v>
       </c>
       <c r="O34" t="n">
-        <v>5.45483296213808</v>
+        <v>0.512180790960452</v>
       </c>
     </row>
     <row r="35">
@@ -3281,13 +3281,13 @@
         <v>75.6283783783784</v>
       </c>
       <c r="M35" t="n">
-        <v>5.62621832358674</v>
+        <v>0.555877237851662</v>
       </c>
       <c r="N35" t="n">
-        <v>4.17857699805068</v>
+        <v>0.436539641943734</v>
       </c>
       <c r="O35" t="n">
-        <v>5.53198830409357</v>
+        <v>0.495030690537084</v>
       </c>
     </row>
     <row r="36">
@@ -3328,13 +3328,13 @@
         <v>64.8715277777778</v>
       </c>
       <c r="M36" t="n">
-        <v>5.84589068825911</v>
+        <v>0.584745945945946</v>
       </c>
       <c r="N36" t="n">
-        <v>4.05176113360324</v>
+        <v>0.410778378378379</v>
       </c>
       <c r="O36" t="n">
-        <v>5.6082995951417</v>
+        <v>0.4768</v>
       </c>
     </row>
     <row r="37">
@@ -3372,16 +3372,16 @@
         <v>0.525152194809356</v>
       </c>
       <c r="L37" t="n">
-        <v>120.670041454082</v>
+        <v>122.854070286503</v>
       </c>
       <c r="M37" t="n">
-        <v>5.96134113411341</v>
+        <v>0.607322195704057</v>
       </c>
       <c r="N37" t="n">
-        <v>4.08474347434743</v>
+        <v>0.395403341288782</v>
       </c>
       <c r="O37" t="n">
-        <v>5.64000900090009</v>
+        <v>0.45927446300716</v>
       </c>
     </row>
     <row r="38">
@@ -3422,13 +3422,13 @@
         <v>95.9216326530612</v>
       </c>
       <c r="M38" t="n">
-        <v>5.64734426229508</v>
+        <v>0.56481007751938</v>
       </c>
       <c r="N38" t="n">
-        <v>4.18783606557377</v>
+        <v>0.452732558139535</v>
       </c>
       <c r="O38" t="n">
-        <v>5.48285245901639</v>
+        <v>0.480089147286822</v>
       </c>
     </row>
     <row r="39">
@@ -3469,13 +3469,13 @@
         <v>78.4824943849914</v>
       </c>
       <c r="M39" t="n">
-        <v>5.8455325443787</v>
+        <v>0.604796477495107</v>
       </c>
       <c r="N39" t="n">
-        <v>4.17269230769231</v>
+        <v>0.452577299412916</v>
       </c>
       <c r="O39" t="n">
-        <v>5.60402366863905</v>
+        <v>0.52733072407045</v>
       </c>
     </row>
     <row r="40">
@@ -3516,13 +3516,13 @@
         <v>145.187641723356</v>
       </c>
       <c r="M40" t="n">
-        <v>5.82398832684825</v>
+        <v>0.611367088607594</v>
       </c>
       <c r="N40" t="n">
-        <v>4.05540856031128</v>
+        <v>0.428946835443038</v>
       </c>
       <c r="O40" t="n">
-        <v>5.58941634241245</v>
+        <v>0.510384810126583</v>
       </c>
     </row>
     <row r="41">
@@ -3563,13 +3563,13 @@
         <v>80.8806818181818</v>
       </c>
       <c r="M41" t="n">
-        <v>5.86301369863014</v>
+        <v>0.623990825688073</v>
       </c>
       <c r="N41" t="n">
-        <v>4.10743150684931</v>
+        <v>0.412394495412844</v>
       </c>
       <c r="O41" t="n">
-        <v>5.67380136986301</v>
+        <v>0.455536697247706</v>
       </c>
     </row>
     <row r="42">
@@ -3610,13 +3610,13 @@
         <v>43.2012</v>
       </c>
       <c r="M42" t="n">
-        <v>5.75175862068965</v>
+        <v>0.582337209302326</v>
       </c>
       <c r="N42" t="n">
-        <v>4.1368275862069</v>
+        <v>0.460874418604651</v>
       </c>
       <c r="O42" t="n">
-        <v>5.60408620689655</v>
+        <v>0.507506976744186</v>
       </c>
     </row>
     <row r="43">
@@ -3648,22 +3648,22 @@
         <v>45.1672862453532</v>
       </c>
       <c r="J43" t="n">
-        <v>0.468661417322835</v>
+        <v>0.468346456692913</v>
       </c>
       <c r="K43" t="n">
-        <v>0.531338582677165</v>
+        <v>0.531653543307087</v>
       </c>
       <c r="L43" t="n">
-        <v>72.3531713042203</v>
+        <v>72.1979069881168</v>
       </c>
       <c r="M43" t="n">
-        <v>5.80222596964587</v>
+        <v>0.573014167650527</v>
       </c>
       <c r="N43" t="n">
-        <v>4.05823777403035</v>
+        <v>0.424932703659976</v>
       </c>
       <c r="O43" t="n">
-        <v>5.5710370994941</v>
+        <v>0.464546635183001</v>
       </c>
     </row>
     <row r="44">
@@ -3704,13 +3704,13 @@
         <v>104.039697542533</v>
       </c>
       <c r="M44" t="n">
-        <v>5.79587515299878</v>
+        <v>0.575344773790951</v>
       </c>
       <c r="N44" t="n">
-        <v>4.0852876376989</v>
+        <v>0.44438065522621</v>
       </c>
       <c r="O44" t="n">
-        <v>5.68253365973072</v>
+        <v>0.498017160686427</v>
       </c>
     </row>
     <row r="45">
@@ -3751,13 +3751,13 @@
         <v>93.9752066115703</v>
       </c>
       <c r="M45" t="n">
-        <v>5.93924281984334</v>
+        <v>0.623982269503546</v>
       </c>
       <c r="N45" t="n">
-        <v>4.15694516971279</v>
+        <v>0.435258865248226</v>
       </c>
       <c r="O45" t="n">
-        <v>5.59349869451697</v>
+        <v>0.499276595744681</v>
       </c>
     </row>
     <row r="46">
@@ -3798,13 +3798,13 @@
         <v>98.9049123814996</v>
       </c>
       <c r="M46" t="n">
-        <v>5.79339694656488</v>
+        <v>0.590118518518519</v>
       </c>
       <c r="N46" t="n">
-        <v>4.17049618320611</v>
+        <v>0.42623950617284</v>
       </c>
       <c r="O46" t="n">
-        <v>5.54673664122137</v>
+        <v>0.472032098765432</v>
       </c>
     </row>
     <row r="47">
@@ -3845,13 +3845,13 @@
         <v>87.3656804733728</v>
       </c>
       <c r="M47" t="n">
-        <v>5.90048824593128</v>
+        <v>0.602796440489432</v>
       </c>
       <c r="N47" t="n">
-        <v>4.12978300180832</v>
+        <v>0.443669632925474</v>
       </c>
       <c r="O47" t="n">
-        <v>5.62773056057866</v>
+        <v>0.511901001112348</v>
       </c>
     </row>
     <row r="48">
@@ -3892,13 +3892,13 @@
         <v>102.148760330578</v>
       </c>
       <c r="M48" t="n">
-        <v>5.74587400177462</v>
+        <v>0.583020334928231</v>
       </c>
       <c r="N48" t="n">
-        <v>4.19927684117125</v>
+        <v>0.460669258373207</v>
       </c>
       <c r="O48" t="n">
-        <v>5.53271517302573</v>
+        <v>0.513864234449762</v>
       </c>
     </row>
     <row r="49">
@@ -3939,13 +3939,13 @@
         <v>140.652366863905</v>
       </c>
       <c r="M49" t="n">
-        <v>5.7456890459364</v>
+        <v>0.573028436018957</v>
       </c>
       <c r="N49" t="n">
-        <v>4.03095406360424</v>
+        <v>0.383957345971564</v>
       </c>
       <c r="O49" t="n">
-        <v>5.64996466431095</v>
+        <v>0.482530805687204</v>
       </c>
     </row>
     <row r="50">
@@ -3983,16 +3983,16 @@
         <v>0.520628683693517</v>
       </c>
       <c r="L50" t="n">
-        <v>83.0805785123967</v>
+        <v>82.5547520661157</v>
       </c>
       <c r="M50" t="n">
-        <v>5.88727979274611</v>
+        <v>0.571711267605634</v>
       </c>
       <c r="N50" t="n">
-        <v>4.03007772020725</v>
+        <v>0.422257042253522</v>
       </c>
       <c r="O50" t="n">
-        <v>5.52966321243523</v>
+        <v>0.49163028169014</v>
       </c>
     </row>
     <row r="51">
@@ -4024,22 +4024,22 @@
         <v>47.2972972972973</v>
       </c>
       <c r="J51" t="n">
-        <v>0.455752212389381</v>
+        <v>0.45575221238938</v>
       </c>
       <c r="K51" t="n">
         <v>0.544247787610619</v>
       </c>
       <c r="L51" t="n">
-        <v>126.033293697979</v>
+        <v>125.563020214031</v>
       </c>
       <c r="M51" t="n">
-        <v>5.93018315018315</v>
+        <v>0.596911270983213</v>
       </c>
       <c r="N51" t="n">
-        <v>4.14727106227106</v>
+        <v>0.418163069544364</v>
       </c>
       <c r="O51" t="n">
-        <v>5.65360805860806</v>
+        <v>0.469585131894484</v>
       </c>
     </row>
     <row r="52">
@@ -4080,13 +4080,13 @@
         <v>95.2377225097841</v>
       </c>
       <c r="M52" t="n">
-        <v>6.04337679269883</v>
+        <v>0.62472520325203</v>
       </c>
       <c r="N52" t="n">
-        <v>4.11717079530639</v>
+        <v>0.438967479674797</v>
       </c>
       <c r="O52" t="n">
-        <v>5.75044328552803</v>
+        <v>0.506613008130081</v>
       </c>
     </row>
     <row r="53">
@@ -4127,13 +4127,13 @@
         <v>43.42</v>
       </c>
       <c r="M53" t="n">
-        <v>5.92951327433628</v>
+        <v>0.612</v>
       </c>
       <c r="N53" t="n">
-        <v>3.87800884955752</v>
+        <v>0.383345911949685</v>
       </c>
       <c r="O53" t="n">
-        <v>5.63991150442478</v>
+        <v>0.402433962264151</v>
       </c>
     </row>
     <row r="54">
@@ -4174,13 +4174,13 @@
         <v>91.1720235400634</v>
       </c>
       <c r="M54" t="n">
-        <v>5.88798866855524</v>
+        <v>0.6211</v>
       </c>
       <c r="N54" t="n">
-        <v>4.21351274787535</v>
+        <v>0.482337931034483</v>
       </c>
       <c r="O54" t="n">
-        <v>5.65118980169972</v>
+        <v>0.558441379310344</v>
       </c>
     </row>
     <row r="55">
@@ -4221,13 +4221,13 @@
         <v>71.6666666666667</v>
       </c>
       <c r="M55" t="n">
-        <v>5.91421818181818</v>
+        <v>0.62865296803653</v>
       </c>
       <c r="N55" t="n">
-        <v>4.06807272727273</v>
+        <v>0.43237899543379</v>
       </c>
       <c r="O55" t="n">
-        <v>5.5444</v>
+        <v>0.542497716894978</v>
       </c>
     </row>
     <row r="56">
@@ -4268,13 +4268,13 @@
         <v>73.754132231405</v>
       </c>
       <c r="M56" t="n">
-        <v>5.7999696969697</v>
+        <v>0.601948412698413</v>
       </c>
       <c r="N56" t="n">
-        <v>4.20745454545455</v>
+        <v>0.470734126984127</v>
       </c>
       <c r="O56" t="n">
-        <v>5.51</v>
+        <v>0.54375</v>
       </c>
     </row>
     <row r="57">
@@ -4315,13 +4315,13 @@
         <v>78.933518325818</v>
       </c>
       <c r="M57" t="n">
-        <v>5.71854929577465</v>
+        <v>0.574208633093525</v>
       </c>
       <c r="N57" t="n">
-        <v>4.09256338028169</v>
+        <v>0.462908273381295</v>
       </c>
       <c r="O57" t="n">
-        <v>5.61578873239437</v>
+        <v>0.524996402877698</v>
       </c>
     </row>
     <row r="58">
@@ -4362,13 +4362,13 @@
         <v>68.7407407407407</v>
       </c>
       <c r="M58" t="n">
-        <v>5.7778125</v>
+        <v>0.57646017699115</v>
       </c>
       <c r="N58" t="n">
-        <v>4.099453125</v>
+        <v>0.469805309734513</v>
       </c>
       <c r="O58" t="n">
-        <v>5.659296875</v>
+        <v>0.50258407079646</v>
       </c>
     </row>
     <row r="59">
@@ -4409,13 +4409,13 @@
         <v>122.3349609375</v>
       </c>
       <c r="M59" t="n">
-        <v>5.89985576923077</v>
+        <v>0.626991631799163</v>
       </c>
       <c r="N59" t="n">
-        <v>4.21895833333333</v>
+        <v>0.474826359832636</v>
       </c>
       <c r="O59" t="n">
-        <v>5.65924679487179</v>
+        <v>0.54173640167364</v>
       </c>
     </row>
     <row r="60">
@@ -4456,13 +4456,13 @@
         <v>82.9752066115702</v>
       </c>
       <c r="M60" t="n">
-        <v>5.54443181818182</v>
+        <v>0.579432835820896</v>
       </c>
       <c r="N60" t="n">
-        <v>3.88659090909091</v>
+        <v>0.366701492537313</v>
       </c>
       <c r="O60" t="n">
-        <v>5.52875</v>
+        <v>0.428149253731343</v>
       </c>
     </row>
     <row r="61">
@@ -4503,13 +4503,13 @@
         <v>140.06</v>
       </c>
       <c r="M61" t="n">
-        <v>5.76069306930693</v>
+        <v>0.546894736842105</v>
       </c>
       <c r="N61" t="n">
-        <v>4.04237623762376</v>
+        <v>0.440434210526316</v>
       </c>
       <c r="O61" t="n">
-        <v>5.5660396039604</v>
+        <v>0.484736842105263</v>
       </c>
     </row>
     <row r="62">
@@ -4550,13 +4550,13 @@
         <v>57.0133121518631</v>
       </c>
       <c r="M62" t="n">
-        <v>5.78489002932551</v>
+        <v>0.606737918215615</v>
       </c>
       <c r="N62" t="n">
-        <v>4.13744134897361</v>
+        <v>0.426253717472119</v>
       </c>
       <c r="O62" t="n">
-        <v>5.64057184750733</v>
+        <v>0.499622676579926</v>
       </c>
     </row>
     <row r="63">
@@ -4597,13 +4597,13 @@
         <v>62.883</v>
       </c>
       <c r="M63" t="n">
-        <v>5.85598240469208</v>
+        <v>0.594778359511343</v>
       </c>
       <c r="N63" t="n">
-        <v>4.05067448680352</v>
+        <v>0.432237347294939</v>
       </c>
       <c r="O63" t="n">
-        <v>5.65595307917889</v>
+        <v>0.482184991273997</v>
       </c>
     </row>
     <row r="64">
@@ -4644,13 +4644,13 @@
         <v>86.6759002770083</v>
       </c>
       <c r="M64" t="n">
-        <v>5.81987341772152</v>
+        <v>0.64366129032258</v>
       </c>
       <c r="N64" t="n">
-        <v>3.99740506329114</v>
+        <v>0.397887096774194</v>
       </c>
       <c r="O64" t="n">
-        <v>5.63139240506329</v>
+        <v>0.496298387096774</v>
       </c>
     </row>
     <row r="65">
@@ -4691,13 +4691,13 @@
         <v>72.3239603024575</v>
       </c>
       <c r="M65" t="n">
-        <v>5.97316473988439</v>
+        <v>0.627558011049723</v>
       </c>
       <c r="N65" t="n">
-        <v>4.19145953757225</v>
+        <v>0.448740331491714</v>
       </c>
       <c r="O65" t="n">
-        <v>5.69238439306358</v>
+        <v>0.513305709023941</v>
       </c>
     </row>
     <row r="66">
@@ -4738,13 +4738,13 @@
         <v>148.165289256198</v>
       </c>
       <c r="M66" t="n">
-        <v>6.01732997481108</v>
+        <v>0.625828885400315</v>
       </c>
       <c r="N66" t="n">
-        <v>4.1444080604534</v>
+        <v>0.442773940345369</v>
       </c>
       <c r="O66" t="n">
-        <v>5.59656171284635</v>
+        <v>0.510794348508633</v>
       </c>
     </row>
     <row r="67">
@@ -4785,13 +4785,13 @@
         <v>139.128888888889</v>
       </c>
       <c r="M67" t="n">
-        <v>5.82746719160105</v>
+        <v>0.576325914149442</v>
       </c>
       <c r="N67" t="n">
-        <v>4.12897637795276</v>
+        <v>0.442238473767886</v>
       </c>
       <c r="O67" t="n">
-        <v>5.62220472440945</v>
+        <v>0.500890302066773</v>
       </c>
     </row>
     <row r="68">
@@ -4829,16 +4829,16 @@
         <v>0.555447470817121</v>
       </c>
       <c r="L68" t="n">
-        <v>89.4177514792899</v>
+        <v>89.41775147929</v>
       </c>
       <c r="M68" t="n">
-        <v>5.7685394352483</v>
+        <v>0.594241011984021</v>
       </c>
       <c r="N68" t="n">
-        <v>4.04452775073028</v>
+        <v>0.429806924101198</v>
       </c>
       <c r="O68" t="n">
-        <v>5.61120740019474</v>
+        <v>0.520126498002663</v>
       </c>
     </row>
     <row r="69">
@@ -4879,13 +4879,13 @@
         <v>149.7125</v>
       </c>
       <c r="M69" t="n">
-        <v>5.91702054794521</v>
+        <v>0.581714634146341</v>
       </c>
       <c r="N69" t="n">
-        <v>4.08645547945205</v>
+        <v>0.432068292682927</v>
       </c>
       <c r="O69" t="n">
-        <v>5.60623287671233</v>
+        <v>0.494470731707317</v>
       </c>
     </row>
     <row r="70">
@@ -4926,13 +4926,13 @@
         <v>102.430989583333</v>
       </c>
       <c r="M70" t="n">
-        <v>5.85925465838509</v>
+        <v>0.601882258064516</v>
       </c>
       <c r="N70" t="n">
-        <v>4.11191304347826</v>
+        <v>0.422109677419355</v>
       </c>
       <c r="O70" t="n">
-        <v>5.64198757763975</v>
+        <v>0.513662903225807</v>
       </c>
     </row>
     <row r="71">
@@ -4973,13 +4973,13 @@
         <v>93.6666666666667</v>
       </c>
       <c r="M71" t="n">
-        <v>5.92413073713491</v>
+        <v>0.593260787992494</v>
       </c>
       <c r="N71" t="n">
-        <v>4.04488178025035</v>
+        <v>0.42031894934334</v>
       </c>
       <c r="O71" t="n">
-        <v>5.66716272600835</v>
+        <v>0.495373358348968</v>
       </c>
     </row>
     <row r="72">
@@ -5020,13 +5020,13 @@
         <v>133.210303729335</v>
       </c>
       <c r="M72" t="n">
-        <v>5.7341978021978</v>
+        <v>0.607235632183908</v>
       </c>
       <c r="N72" t="n">
-        <v>4.04397802197802</v>
+        <v>0.444051724137931</v>
       </c>
       <c r="O72" t="n">
-        <v>5.58505494505494</v>
+        <v>0.52391091954023</v>
       </c>
     </row>
     <row r="73">
@@ -5067,13 +5067,13 @@
         <v>65.3862633900441</v>
       </c>
       <c r="M73" t="n">
-        <v>5.94976608187134</v>
+        <v>0.620275956284153</v>
       </c>
       <c r="N73" t="n">
-        <v>4.14317738791423</v>
+        <v>0.430978142076503</v>
       </c>
       <c r="O73" t="n">
-        <v>5.6316179337232</v>
+        <v>0.518986338797814</v>
       </c>
     </row>
     <row r="74">
@@ -5114,13 +5114,13 @@
         <v>101.001040582726</v>
       </c>
       <c r="M74" t="n">
-        <v>5.750825</v>
+        <v>0.601494233937397</v>
       </c>
       <c r="N74" t="n">
-        <v>4.2236875</v>
+        <v>0.44773805601318</v>
       </c>
       <c r="O74" t="n">
-        <v>5.53705</v>
+        <v>0.53599176276771</v>
       </c>
     </row>
     <row r="75">
@@ -5161,13 +5161,13 @@
         <v>55.8340950154108</v>
       </c>
       <c r="M75" t="n">
-        <v>5.90680327868852</v>
+        <v>0.604555555555555</v>
       </c>
       <c r="N75" t="n">
-        <v>4.14655737704918</v>
+        <v>0.431494758909854</v>
       </c>
       <c r="O75" t="n">
-        <v>5.69155737704918</v>
+        <v>0.526834381551363</v>
       </c>
     </row>
     <row r="76">
@@ -5208,13 +5208,13 @@
         <v>80.7134502923977</v>
       </c>
       <c r="M76" t="n">
-        <v>5.52833333333333</v>
+        <v>0.550017341040462</v>
       </c>
       <c r="N76" t="n">
-        <v>4.20881278538813</v>
+        <v>0.460838150289018</v>
       </c>
       <c r="O76" t="n">
-        <v>5.56926940639269</v>
+        <v>0.507939306358381</v>
       </c>
     </row>
     <row r="77">
@@ -5255,13 +5255,13 @@
         <v>90.7844387755102</v>
       </c>
       <c r="M77" t="n">
-        <v>5.74134897360704</v>
+        <v>0.55634862385321</v>
       </c>
       <c r="N77" t="n">
-        <v>4.14090909090909</v>
+        <v>0.4411376146789</v>
       </c>
       <c r="O77" t="n">
-        <v>5.63973607038123</v>
+        <v>0.499</v>
       </c>
     </row>
     <row r="78">
@@ -5302,13 +5302,13 @@
         <v>100.566837107378</v>
       </c>
       <c r="M78" t="n">
-        <v>5.57944134078212</v>
+        <v>0.54218819188192</v>
       </c>
       <c r="N78" t="n">
-        <v>4.2327094972067</v>
+        <v>0.477070110701107</v>
       </c>
       <c r="O78" t="n">
-        <v>5.32606145251397</v>
+        <v>0.504915129151292</v>
       </c>
     </row>
     <row r="79">
@@ -5349,13 +5349,13 @@
         <v>214.122448979592</v>
       </c>
       <c r="M79" t="n">
-        <v>6.15647619047619</v>
+        <v>0.580405063291139</v>
       </c>
       <c r="N79" t="n">
-        <v>4.17485714285714</v>
+        <v>0.357962025316456</v>
       </c>
       <c r="O79" t="n">
-        <v>5.76780952380952</v>
+        <v>0.427949367088608</v>
       </c>
     </row>
     <row r="80">
@@ -5396,13 +5396,13 @@
         <v>79.6493055555556</v>
       </c>
       <c r="M80" t="n">
-        <v>5.90300934579439</v>
+        <v>0.628722891566265</v>
       </c>
       <c r="N80" t="n">
-        <v>3.99955140186916</v>
+        <v>0.419315662650603</v>
       </c>
       <c r="O80" t="n">
-        <v>5.67097196261682</v>
+        <v>0.503457831325302</v>
       </c>
     </row>
     <row r="81">
@@ -5425,7 +5425,7 @@
         <v>17</v>
       </c>
       <c r="G81" t="n">
-        <v>7.81825917780409</v>
+        <v>7.8182591778041</v>
       </c>
       <c r="H81" t="n">
         <v>0.66</v>
@@ -5443,13 +5443,13 @@
         <v>74.5255198487713</v>
       </c>
       <c r="M81" t="n">
-        <v>5.77254054054054</v>
+        <v>0.57895652173913</v>
       </c>
       <c r="N81" t="n">
-        <v>4.11513513513513</v>
+        <v>0.401826086956522</v>
       </c>
       <c r="O81" t="n">
-        <v>5.44978378378378</v>
+        <v>0.444726708074534</v>
       </c>
     </row>
     <row r="82">
@@ -5490,13 +5490,13 @@
         <v>75.6633714880333</v>
       </c>
       <c r="M82" t="n">
-        <v>5.99714285714286</v>
+        <v>0.60096511627907</v>
       </c>
       <c r="N82" t="n">
-        <v>4.02837053571429</v>
+        <v>0.396502906976744</v>
       </c>
       <c r="O82" t="n">
-        <v>5.74017857142857</v>
+        <v>0.469101744186046</v>
       </c>
     </row>
     <row r="83">
@@ -5537,13 +5537,13 @@
         <v>78.1933778355388</v>
       </c>
       <c r="M83" t="n">
-        <v>5.78185426154847</v>
+        <v>0.584750994431184</v>
       </c>
       <c r="N83" t="n">
-        <v>4.05389720234222</v>
+        <v>0.411933174224345</v>
       </c>
       <c r="O83" t="n">
-        <v>5.6371372804164</v>
+        <v>0.499400159108991</v>
       </c>
     </row>
     <row r="84">
@@ -5575,22 +5575,22 @@
         <v>51.0344827586207</v>
       </c>
       <c r="J84" t="n">
-        <v>0.450446218882104</v>
+        <v>0.449976514795679</v>
       </c>
       <c r="K84" t="n">
-        <v>0.549553781117896</v>
+        <v>0.550023485204321</v>
       </c>
       <c r="L84" t="n">
         <v>122.476988823143</v>
       </c>
       <c r="M84" t="n">
-        <v>5.89802710843373</v>
+        <v>0.594446927374302</v>
       </c>
       <c r="N84" t="n">
-        <v>4.16495481927711</v>
+        <v>0.460981378026071</v>
       </c>
       <c r="O84" t="n">
-        <v>5.64149096385542</v>
+        <v>0.521173184357542</v>
       </c>
     </row>
     <row r="85">
@@ -5631,13 +5631,13 @@
         <v>202.959183673469</v>
       </c>
       <c r="M85" t="n">
-        <v>5.67522222222222</v>
+        <v>0.573</v>
       </c>
       <c r="N85" t="n">
-        <v>4.00922222222222</v>
+        <v>0.387550724637682</v>
       </c>
       <c r="O85" t="n">
-        <v>5.42655555555556</v>
+        <v>0.45368115942029</v>
       </c>
     </row>
     <row r="86">
@@ -5678,13 +5678,13 @@
         <v>112.71048553719</v>
       </c>
       <c r="M86" t="n">
-        <v>5.74988188976378</v>
+        <v>0.594247833622183</v>
       </c>
       <c r="N86" t="n">
-        <v>4.20086614173228</v>
+        <v>0.449461005199306</v>
       </c>
       <c r="O86" t="n">
-        <v>5.67439632545932</v>
+        <v>0.533207972270365</v>
       </c>
     </row>
     <row r="87">
@@ -5725,13 +5725,13 @@
         <v>83.1780185079602</v>
       </c>
       <c r="M87" t="n">
-        <v>5.87941376380629</v>
+        <v>0.616962921348314</v>
       </c>
       <c r="N87" t="n">
-        <v>4.02823279524214</v>
+        <v>0.414442696629215</v>
       </c>
       <c r="O87" t="n">
-        <v>5.65407816482583</v>
+        <v>0.511485393258428</v>
       </c>
     </row>
     <row r="88">
@@ -5772,13 +5772,13 @@
         <v>73.9135841836735</v>
       </c>
       <c r="M88" t="n">
-        <v>5.82892420537897</v>
+        <v>0.566635014836796</v>
       </c>
       <c r="N88" t="n">
-        <v>4.11110024449878</v>
+        <v>0.426543026706232</v>
       </c>
       <c r="O88" t="n">
-        <v>5.65002444987775</v>
+        <v>0.479142433234421</v>
       </c>
     </row>
     <row r="89">
@@ -5819,13 +5819,13 @@
         <v>122.6225</v>
       </c>
       <c r="M89" t="n">
-        <v>5.86901639344262</v>
+        <v>0.643595890410958</v>
       </c>
       <c r="N89" t="n">
-        <v>4.32666666666667</v>
+        <v>0.443582191780822</v>
       </c>
       <c r="O89" t="n">
-        <v>5.63606557377049</v>
+        <v>0.549424657534246</v>
       </c>
     </row>
     <row r="90">
@@ -5866,13 +5866,13 @@
         <v>81.9705175452652</v>
       </c>
       <c r="M90" t="n">
-        <v>5.64651125401929</v>
+        <v>0.548922155688622</v>
       </c>
       <c r="N90" t="n">
-        <v>4.15606109324759</v>
+        <v>0.434347305389222</v>
       </c>
       <c r="O90" t="n">
-        <v>5.5553536977492</v>
+        <v>0.485656686626747</v>
       </c>
     </row>
     <row r="91">
@@ -5913,13 +5913,13 @@
         <v>187.6875</v>
       </c>
       <c r="M91" t="n">
-        <v>5.76125</v>
+        <v>0.585846153846154</v>
       </c>
       <c r="N91" t="n">
-        <v>4.00725</v>
+        <v>0.418974358974359</v>
       </c>
       <c r="O91" t="n">
-        <v>5.59775</v>
+        <v>0.524666666666667</v>
       </c>
     </row>
     <row r="92">
@@ -5960,13 +5960,13 @@
         <v>88.8168714555766</v>
       </c>
       <c r="M92" t="n">
-        <v>5.79055412371134</v>
+        <v>0.592499148211242</v>
       </c>
       <c r="N92" t="n">
-        <v>4.17239690721649</v>
+        <v>0.459473594548552</v>
       </c>
       <c r="O92" t="n">
-        <v>5.59778350515464</v>
+        <v>0.523710391822827</v>
       </c>
     </row>
     <row r="93">
@@ -6007,13 +6007,13 @@
         <v>93.4857335241141</v>
       </c>
       <c r="M93" t="n">
-        <v>5.74874572405929</v>
+        <v>0.5943095599393</v>
       </c>
       <c r="N93" t="n">
-        <v>4.11842645381984</v>
+        <v>0.434538694992413</v>
       </c>
       <c r="O93" t="n">
-        <v>5.59071835803877</v>
+        <v>0.49313808801214</v>
       </c>
     </row>
     <row r="94">
@@ -6054,13 +6054,13 @@
         <v>101.144631117604</v>
       </c>
       <c r="M94" t="n">
-        <v>5.98328358208955</v>
+        <v>0.609902040816326</v>
       </c>
       <c r="N94" t="n">
-        <v>3.98970149253731</v>
+        <v>0.389216326530612</v>
       </c>
       <c r="O94" t="n">
-        <v>5.69229850746269</v>
+        <v>0.484722448979591</v>
       </c>
     </row>
     <row r="95">
@@ -6101,13 +6101,13 @@
         <v>99.3431952662722</v>
       </c>
       <c r="M95" t="n">
-        <v>5.9834703196347</v>
+        <v>0.612017341040463</v>
       </c>
       <c r="N95" t="n">
-        <v>4.0772602739726</v>
+        <v>0.427052023121387</v>
       </c>
       <c r="O95" t="n">
-        <v>5.67662100456621</v>
+        <v>0.536537572254336</v>
       </c>
     </row>
     <row r="96">
@@ -6148,13 +6148,13 @@
         <v>78.8360969387755</v>
       </c>
       <c r="M96" t="n">
-        <v>5.72235154394299</v>
+        <v>0.553746987951806</v>
       </c>
       <c r="N96" t="n">
-        <v>4.18301662707839</v>
+        <v>0.476846385542169</v>
       </c>
       <c r="O96" t="n">
-        <v>5.61351543942993</v>
+        <v>0.509253012048193</v>
       </c>
     </row>
     <row r="97">
@@ -6195,13 +6195,13 @@
         <v>71.3304662743323</v>
       </c>
       <c r="M97" t="n">
-        <v>5.93873524451939</v>
+        <v>0.614572062084257</v>
       </c>
       <c r="N97" t="n">
-        <v>4.10822934232715</v>
+        <v>0.427643015521065</v>
       </c>
       <c r="O97" t="n">
-        <v>5.69377740303541</v>
+        <v>0.503756097560975</v>
       </c>
     </row>
     <row r="98">
@@ -6242,13 +6242,13 @@
         <v>92.0106267359015</v>
       </c>
       <c r="M98" t="n">
-        <v>5.91469230769231</v>
+        <v>0.609670967741934</v>
       </c>
       <c r="N98" t="n">
-        <v>4.09138461538462</v>
+        <v>0.431314516129032</v>
       </c>
       <c r="O98" t="n">
-        <v>5.60303846153846</v>
+        <v>0.506011290322581</v>
       </c>
     </row>
     <row r="99">
@@ -6289,13 +6289,13 @@
         <v>91.1561595010024</v>
       </c>
       <c r="M99" t="n">
-        <v>5.79996197718631</v>
+        <v>0.595423558897243</v>
       </c>
       <c r="N99" t="n">
-        <v>4.16134980988593</v>
+        <v>0.454749373433584</v>
       </c>
       <c r="O99" t="n">
-        <v>5.64480988593156</v>
+        <v>0.544278195488721</v>
       </c>
     </row>
     <row r="100">
@@ -6327,22 +6327,22 @@
         <v>47.3577235772358</v>
       </c>
       <c r="J100" t="n">
-        <v>0.480675422138837</v>
+        <v>0.48048048048048</v>
       </c>
       <c r="K100" t="n">
-        <v>0.519324577861163</v>
+        <v>0.519519519519519</v>
       </c>
       <c r="L100" t="n">
-        <v>135.70593100189</v>
+        <v>135.655009451796</v>
       </c>
       <c r="M100" t="n">
-        <v>5.9807725788901</v>
+        <v>0.611821301775146</v>
       </c>
       <c r="N100" t="n">
-        <v>3.98413492927095</v>
+        <v>0.36841775147929</v>
       </c>
       <c r="O100" t="n">
-        <v>5.69096844396083</v>
+        <v>0.467029585798816</v>
       </c>
     </row>
     <row r="101">
@@ -6383,13 +6383,13 @@
         <v>3.38775510204082</v>
       </c>
       <c r="M101" t="n">
-        <v>6.44892857142857</v>
+        <v>0.755837837837838</v>
       </c>
       <c r="N101" t="n">
-        <v>3.80767857142857</v>
+        <v>0.411207207207207</v>
       </c>
       <c r="O101" t="n">
-        <v>5.95080357142857</v>
+        <v>0.569315315315315</v>
       </c>
     </row>
     <row r="102">
@@ -6430,13 +6430,13 @@
         <v>98.8430439952438</v>
       </c>
       <c r="M102" t="n">
-        <v>5.8289696969697</v>
+        <v>0.578142857142857</v>
       </c>
       <c r="N102" t="n">
-        <v>4.13731313131313</v>
+        <v>0.441464985994398</v>
       </c>
       <c r="O102" t="n">
-        <v>5.59141414141414</v>
+        <v>0.504302521008403</v>
       </c>
     </row>
     <row r="103">
@@ -6477,13 +6477,13 @@
         <v>87.5302933673469</v>
       </c>
       <c r="M103" t="n">
-        <v>5.76600422832981</v>
+        <v>0.603344780219779</v>
       </c>
       <c r="N103" t="n">
-        <v>4.09659619450317</v>
+        <v>0.437243131868131</v>
       </c>
       <c r="O103" t="n">
-        <v>5.59459830866808</v>
+        <v>0.508145604395605</v>
       </c>
     </row>
     <row r="104">
@@ -6524,13 +6524,13 @@
         <v>96.9422222222222</v>
       </c>
       <c r="M104" t="n">
-        <v>5.8178407079646</v>
+        <v>0.628090909090908</v>
       </c>
       <c r="N104" t="n">
-        <v>4.1109203539823</v>
+        <v>0.448586363636363</v>
       </c>
       <c r="O104" t="n">
-        <v>5.58863716814159</v>
+        <v>0.516206818181819</v>
       </c>
     </row>
     <row r="105">
@@ -6571,13 +6571,13 @@
         <v>69.681690940809</v>
       </c>
       <c r="M105" t="n">
-        <v>5.82814397224631</v>
+        <v>0.607662735849057</v>
       </c>
       <c r="N105" t="n">
-        <v>4.12556808326106</v>
+        <v>0.454581367924529</v>
       </c>
       <c r="O105" t="n">
-        <v>5.60235039028621</v>
+        <v>0.519682783018868</v>
       </c>
     </row>
     <row r="106">
@@ -6618,13 +6618,13 @@
         <v>81.9313215400624</v>
       </c>
       <c r="M106" t="n">
-        <v>5.81178723404255</v>
+        <v>0.578024390243903</v>
       </c>
       <c r="N106" t="n">
-        <v>4.20417021276596</v>
+        <v>0.44484756097561</v>
       </c>
       <c r="O106" t="n">
-        <v>5.50787234042553</v>
+        <v>0.515256097560976</v>
       </c>
     </row>
     <row r="107">
@@ -6665,13 +6665,13 @@
         <v>37.25</v>
       </c>
       <c r="M107" t="n">
-        <v>5.86551724137931</v>
+        <v>0.593586956521739</v>
       </c>
       <c r="N107" t="n">
-        <v>3.80827586206897</v>
+        <v>0.410239130434783</v>
       </c>
       <c r="O107" t="n">
-        <v>5.43793103448276</v>
+        <v>0.504239130434782</v>
       </c>
     </row>
     <row r="108">
@@ -6712,13 +6712,13 @@
         <v>78.1666666666667</v>
       </c>
       <c r="M108" t="n">
-        <v>5.86911111111111</v>
+        <v>0.591702702702703</v>
       </c>
       <c r="N108" t="n">
-        <v>4.08755555555556</v>
+        <v>0.386432432432432</v>
       </c>
       <c r="O108" t="n">
-        <v>5.60422222222222</v>
+        <v>0.483243243243243</v>
       </c>
     </row>
     <row r="109">
@@ -6759,13 +6759,13 @@
         <v>5.88429752066116</v>
       </c>
       <c r="M109" t="n">
-        <v>5.98204545454545</v>
+        <v>0.6677</v>
       </c>
       <c r="N109" t="n">
-        <v>4.58954545454545</v>
+        <v>0.5181</v>
       </c>
       <c r="O109" t="n">
-        <v>5.35227272727273</v>
+        <v>0.534</v>
       </c>
     </row>
     <row r="110">
@@ -6806,13 +6806,13 @@
         <v>102.861111111111</v>
       </c>
       <c r="M110" t="n">
-        <v>5.94443965517241</v>
+        <v>0.590513513513514</v>
       </c>
       <c r="N110" t="n">
-        <v>4.03301724137931</v>
+        <v>0.382545945945946</v>
       </c>
       <c r="O110" t="n">
-        <v>5.59741379310345</v>
+        <v>0.435967567567567</v>
       </c>
     </row>
     <row r="111">
@@ -6853,13 +6853,13 @@
         <v>96.8737024221453</v>
       </c>
       <c r="M111" t="n">
-        <v>5.87597972972973</v>
+        <v>0.594171052631579</v>
       </c>
       <c r="N111" t="n">
-        <v>4.24202702702703</v>
+        <v>0.445311403508772</v>
       </c>
       <c r="O111" t="n">
-        <v>5.65054054054054</v>
+        <v>0.515570175438597</v>
       </c>
     </row>
     <row r="112">
@@ -6900,13 +6900,13 @@
         <v>38.7222222222222</v>
       </c>
       <c r="M112" t="n">
-        <v>5.60475862068966</v>
+        <v>0.556683333333333</v>
       </c>
       <c r="N112" t="n">
-        <v>4.05820689655172</v>
+        <v>0.42795</v>
       </c>
       <c r="O112" t="n">
-        <v>5.65220689655172</v>
+        <v>0.480875</v>
       </c>
     </row>
     <row r="113">
@@ -6947,13 +6947,13 @@
         <v>63.2128099173554</v>
       </c>
       <c r="M113" t="n">
-        <v>5.98587196467991</v>
+        <v>0.616466480446927</v>
       </c>
       <c r="N113" t="n">
-        <v>4.15741721854305</v>
+        <v>0.465307262569832</v>
       </c>
       <c r="O113" t="n">
-        <v>5.6932229580574</v>
+        <v>0.538513966480446</v>
       </c>
     </row>
     <row r="114">
@@ -6994,13 +6994,13 @@
         <v>208.32</v>
       </c>
       <c r="M114" t="n">
-        <v>5.93931034482759</v>
+        <v>0.609818181818182</v>
       </c>
       <c r="N114" t="n">
-        <v>4.0998275862069</v>
+        <v>0.409181818181818</v>
       </c>
       <c r="O114" t="n">
-        <v>5.55655172413793</v>
+        <v>0.479181818181818</v>
       </c>
     </row>
     <row r="115">
@@ -7041,13 +7041,13 @@
         <v>84.4835069444444</v>
       </c>
       <c r="M115" t="n">
-        <v>5.81706766917293</v>
+        <v>0.609066666666666</v>
       </c>
       <c r="N115" t="n">
-        <v>4.07842105263158</v>
+        <v>0.433279365079365</v>
       </c>
       <c r="O115" t="n">
-        <v>5.70551378446115</v>
+        <v>0.521101587301588</v>
       </c>
     </row>
     <row r="116">
@@ -7088,13 +7088,13 @@
         <v>148.490740740741</v>
       </c>
       <c r="M116" t="n">
-        <v>5.62262886597938</v>
+        <v>0.590562913907285</v>
       </c>
       <c r="N116" t="n">
-        <v>4.25840206185567</v>
+        <v>0.425225165562914</v>
       </c>
       <c r="O116" t="n">
-        <v>5.41685567010309</v>
+        <v>0.516350993377484</v>
       </c>
     </row>
     <row r="117">
@@ -7135,13 +7135,13 @@
         <v>223</v>
       </c>
       <c r="M117" t="n">
-        <v>5.55959459459459</v>
+        <v>0.562153846153846</v>
       </c>
       <c r="N117" t="n">
-        <v>4.04283783783784</v>
+        <v>0.408984615384616</v>
       </c>
       <c r="O117" t="n">
-        <v>5.56797297297297</v>
+        <v>0.503923076923077</v>
       </c>
     </row>
     <row r="118">
@@ -7182,13 +7182,13 @@
         <v>66.1244444444444</v>
       </c>
       <c r="M118" t="n">
-        <v>5.9868992248062</v>
+        <v>0.649797752808989</v>
       </c>
       <c r="N118" t="n">
-        <v>3.87255813953488</v>
+        <v>0.389651685393258</v>
       </c>
       <c r="O118" t="n">
-        <v>5.72046511627907</v>
+        <v>0.559573033707865</v>
       </c>
     </row>
     <row r="119">
@@ -7229,13 +7229,13 @@
         <v>109</v>
       </c>
       <c r="M119" t="n">
-        <v>6.06936936936937</v>
+        <v>0.611458823529412</v>
       </c>
       <c r="N119" t="n">
-        <v>4.0963963963964</v>
+        <v>0.376988235294118</v>
       </c>
       <c r="O119" t="n">
-        <v>5.6036036036036</v>
+        <v>0.451341176470588</v>
       </c>
     </row>
     <row r="120">
@@ -7276,13 +7276,13 @@
         <v>82.8</v>
       </c>
       <c r="M120" t="n">
-        <v>5.96371900826446</v>
+        <v>0.631159090909091</v>
       </c>
       <c r="N120" t="n">
-        <v>4.04504132231405</v>
+        <v>0.373488636363637</v>
       </c>
       <c r="O120" t="n">
-        <v>5.63115702479339</v>
+        <v>0.461556818181818</v>
       </c>
     </row>
     <row r="121">
@@ -7323,13 +7323,13 @@
         <v>158.08</v>
       </c>
       <c r="M121" t="n">
-        <v>6.02488888888889</v>
+        <v>0.67253488372093</v>
       </c>
       <c r="N121" t="n">
-        <v>4.10133333333333</v>
+        <v>0.428139534883721</v>
       </c>
       <c r="O121" t="n">
-        <v>5.93711111111111</v>
+        <v>0.515697674418604</v>
       </c>
     </row>
     <row r="122">
@@ -7370,13 +7370,13 @@
         <v>54.8657024793388</v>
       </c>
       <c r="M122" t="n">
-        <v>5.82811320754717</v>
+        <v>0.607010600706714</v>
       </c>
       <c r="N122" t="n">
-        <v>4.06145552560647</v>
+        <v>0.425173144876325</v>
       </c>
       <c r="O122" t="n">
-        <v>5.4911590296496</v>
+        <v>0.522</v>
       </c>
     </row>
     <row r="123">
@@ -7417,13 +7417,13 @@
         <v>64.2552777777778</v>
       </c>
       <c r="M123" t="n">
-        <v>5.78193480546793</v>
+        <v>0.564473190348526</v>
       </c>
       <c r="N123" t="n">
-        <v>4.10762355415352</v>
+        <v>0.41295710455764</v>
       </c>
       <c r="O123" t="n">
-        <v>5.46652996845426</v>
+        <v>0.453950402144773</v>
       </c>
     </row>
     <row r="124">
@@ -7464,13 +7464,13 @@
         <v>97.8379017013232</v>
       </c>
       <c r="M124" t="n">
-        <v>5.69889265536723</v>
+        <v>0.587661064425769</v>
       </c>
       <c r="N124" t="n">
-        <v>4.07194350282486</v>
+        <v>0.43228431372549</v>
       </c>
       <c r="O124" t="n">
-        <v>5.6059209039548</v>
+        <v>0.509742296918768</v>
       </c>
     </row>
     <row r="125">
@@ -7511,13 +7511,13 @@
         <v>69.7821361058601</v>
       </c>
       <c r="M125" t="n">
-        <v>5.7816081871345</v>
+        <v>0.59453488372093</v>
       </c>
       <c r="N125" t="n">
-        <v>3.98488304093567</v>
+        <v>0.426086378737542</v>
       </c>
       <c r="O125" t="n">
-        <v>5.56766081871345</v>
+        <v>0.469245847176079</v>
       </c>
     </row>
     <row r="126">
@@ -7558,13 +7558,13 @@
         <v>71.3636363636364</v>
       </c>
       <c r="M126" t="n">
-        <v>6.03319474835886</v>
+        <v>0.612242057488654</v>
       </c>
       <c r="N126" t="n">
-        <v>4.00967177242888</v>
+        <v>0.408400907715583</v>
       </c>
       <c r="O126" t="n">
-        <v>5.70823851203501</v>
+        <v>0.497387291981846</v>
       </c>
     </row>
     <row r="127">
@@ -7605,13 +7605,13 @@
         <v>97.8665895336419</v>
       </c>
       <c r="M127" t="n">
-        <v>5.77189247311828</v>
+        <v>0.574171145685996</v>
       </c>
       <c r="N127" t="n">
-        <v>4.06962365591398</v>
+        <v>0.417526166902404</v>
       </c>
       <c r="O127" t="n">
-        <v>5.52447311827957</v>
+        <v>0.488902404526167</v>
       </c>
     </row>
     <row r="128">
@@ -7652,13 +7652,13 @@
         <v>101.399887408519</v>
       </c>
       <c r="M128" t="n">
-        <v>5.85210743801653</v>
+        <v>0.581931589537224</v>
       </c>
       <c r="N128" t="n">
-        <v>4.0396694214876</v>
+        <v>0.397042253521126</v>
       </c>
       <c r="O128" t="n">
-        <v>5.59888429752066</v>
+        <v>0.453219315895372</v>
       </c>
     </row>
     <row r="129">
@@ -7699,13 +7699,13 @@
         <v>47.5318696440858</v>
       </c>
       <c r="M129" t="n">
-        <v>5.81590083798883</v>
+        <v>0.604184772516249</v>
       </c>
       <c r="N129" t="n">
-        <v>4.03761173184358</v>
+        <v>0.412451253481894</v>
       </c>
       <c r="O129" t="n">
-        <v>5.58471368715084</v>
+        <v>0.49663695450325</v>
       </c>
     </row>
     <row r="130">
@@ -7746,13 +7746,13 @@
         <v>57.8355555555556</v>
       </c>
       <c r="M130" t="n">
-        <v>6.01591836734694</v>
+        <v>0.614338541666666</v>
       </c>
       <c r="N130" t="n">
-        <v>3.95459183673469</v>
+        <v>0.377395833333333</v>
       </c>
       <c r="O130" t="n">
-        <v>5.82030612244898</v>
+        <v>0.491848958333333</v>
       </c>
     </row>
     <row r="131">
@@ -7793,13 +7793,13 @@
         <v>60.6301440329218</v>
       </c>
       <c r="M131" t="n">
-        <v>5.85840052015605</v>
+        <v>0.593521381578948</v>
       </c>
       <c r="N131" t="n">
-        <v>3.99665799739922</v>
+        <v>0.4083125</v>
       </c>
       <c r="O131" t="n">
-        <v>5.63950585175553</v>
+        <v>0.480217105263159</v>
       </c>
     </row>
     <row r="132">
@@ -7840,13 +7840,13 @@
         <v>63.664151925078</v>
       </c>
       <c r="M132" t="n">
-        <v>5.40873051224944</v>
+        <v>0.506068656716418</v>
       </c>
       <c r="N132" t="n">
-        <v>4.15886414253898</v>
+        <v>0.465417910447762</v>
       </c>
       <c r="O132" t="n">
-        <v>5.43971046770601</v>
+        <v>0.466325373134328</v>
       </c>
     </row>
     <row r="133">
@@ -7887,13 +7887,13 @@
         <v>78.0969444444444</v>
       </c>
       <c r="M133" t="n">
-        <v>5.81375</v>
+        <v>0.595753481894149</v>
       </c>
       <c r="N133" t="n">
-        <v>4.02845833333333</v>
+        <v>0.416410863509749</v>
       </c>
       <c r="O133" t="n">
-        <v>5.60975</v>
+        <v>0.493853760445683</v>
       </c>
     </row>
     <row r="134">
@@ -7934,13 +7934,13 @@
         <v>90.2548148148148</v>
       </c>
       <c r="M134" t="n">
-        <v>5.91916049382716</v>
+        <v>0.623003448275863</v>
       </c>
       <c r="N134" t="n">
-        <v>4.0838024691358</v>
+        <v>0.408299999999999</v>
       </c>
       <c r="O134" t="n">
-        <v>5.65325925925926</v>
+        <v>0.492493103448276</v>
       </c>
     </row>
     <row r="135">
@@ -7981,13 +7981,13 @@
         <v>93.0363636363636</v>
       </c>
       <c r="M135" t="n">
-        <v>5.80357647058824</v>
+        <v>0.584802359882006</v>
       </c>
       <c r="N135" t="n">
-        <v>4.11265882352941</v>
+        <v>0.44965191740413</v>
       </c>
       <c r="O135" t="n">
-        <v>5.58108235294118</v>
+        <v>0.521156342182891</v>
       </c>
     </row>
     <row r="136">
@@ -8028,13 +8028,13 @@
         <v>79.0647694364001</v>
       </c>
       <c r="M136" t="n">
-        <v>5.57349721706865</v>
+        <v>0.552065573770491</v>
       </c>
       <c r="N136" t="n">
-        <v>4.06176252319109</v>
+        <v>0.424138173302107</v>
       </c>
       <c r="O136" t="n">
-        <v>5.45200371057514</v>
+        <v>0.48330093676815</v>
       </c>
     </row>
     <row r="137">
@@ -8075,13 +8075,13 @@
         <v>54.4813181171089</v>
       </c>
       <c r="M137" t="n">
-        <v>5.85826743350108</v>
+        <v>0.593862616822431</v>
       </c>
       <c r="N137" t="n">
-        <v>4.09365204888569</v>
+        <v>0.440123364485982</v>
       </c>
       <c r="O137" t="n">
-        <v>5.68406182602444</v>
+        <v>0.493098130841122</v>
       </c>
     </row>
     <row r="138">
@@ -8122,13 +8122,13 @@
         <v>73.47</v>
       </c>
       <c r="M138" t="n">
-        <v>5.52649350649351</v>
+        <v>0.554435483870968</v>
       </c>
       <c r="N138" t="n">
-        <v>4.08441558441558</v>
+        <v>0.412048387096774</v>
       </c>
       <c r="O138" t="n">
-        <v>5.40051948051948</v>
+        <v>0.467338709677419</v>
       </c>
     </row>
     <row r="139">
@@ -8169,13 +8169,13 @@
         <v>107.466181061394</v>
       </c>
       <c r="M139" t="n">
-        <v>5.77883534136546</v>
+        <v>0.59138775510204</v>
       </c>
       <c r="N139" t="n">
-        <v>4.06373493975904</v>
+        <v>0.429627551020408</v>
       </c>
       <c r="O139" t="n">
-        <v>5.63353413654619</v>
+        <v>0.499229591836735</v>
       </c>
     </row>
     <row r="140">
@@ -8216,13 +8216,13 @@
         <v>95.4126554894538</v>
       </c>
       <c r="M140" t="n">
-        <v>5.74717223650386</v>
+        <v>0.596965299684542</v>
       </c>
       <c r="N140" t="n">
-        <v>4.23259640102828</v>
+        <v>0.457678233438486</v>
       </c>
       <c r="O140" t="n">
-        <v>5.49640102827763</v>
+        <v>0.522652996845426</v>
       </c>
     </row>
     <row r="141">
@@ -8263,13 +8263,13 @@
         <v>66.862</v>
       </c>
       <c r="M141" t="n">
-        <v>5.73481792717087</v>
+        <v>0.591819444444444</v>
       </c>
       <c r="N141" t="n">
-        <v>4.0556862745098</v>
+        <v>0.423463541666668</v>
       </c>
       <c r="O141" t="n">
-        <v>5.61796918767507</v>
+        <v>0.503223958333335</v>
       </c>
     </row>
     <row r="142">
@@ -8310,13 +8310,13 @@
         <v>69.9120661157025</v>
       </c>
       <c r="M142" t="n">
-        <v>5.88693506493506</v>
+        <v>0.596719298245614</v>
       </c>
       <c r="N142" t="n">
-        <v>4.15072727272727</v>
+        <v>0.393098245614035</v>
       </c>
       <c r="O142" t="n">
-        <v>5.58584415584416</v>
+        <v>0.457168421052631</v>
       </c>
     </row>
     <row r="143">
@@ -8357,13 +8357,13 @@
         <v>66.2382271468144</v>
       </c>
       <c r="M143" t="n">
-        <v>6.09727941176471</v>
+        <v>0.627663636363637</v>
       </c>
       <c r="N143" t="n">
-        <v>4.12676470588235</v>
+        <v>0.407145454545454</v>
       </c>
       <c r="O143" t="n">
-        <v>5.61014705882353</v>
+        <v>0.513890909090909</v>
       </c>
     </row>
     <row r="144">
@@ -8404,13 +8404,13 @@
         <v>51.6666666666667</v>
       </c>
       <c r="M144" t="n">
-        <v>6.28984615384615</v>
+        <v>0.687452830188679</v>
       </c>
       <c r="N144" t="n">
-        <v>4.16538461538462</v>
+        <v>0.374245283018868</v>
       </c>
       <c r="O144" t="n">
-        <v>5.77861538461539</v>
+        <v>0.492245283018868</v>
       </c>
     </row>
     <row r="145">
@@ -8451,13 +8451,13 @@
         <v>70.5406427221172</v>
       </c>
       <c r="M145" t="n">
-        <v>5.6632</v>
+        <v>0.589787878787879</v>
       </c>
       <c r="N145" t="n">
-        <v>4.08971428571429</v>
+        <v>0.388431818181818</v>
       </c>
       <c r="O145" t="n">
-        <v>5.48331428571429</v>
+        <v>0.465136363636364</v>
       </c>
     </row>
     <row r="146">
@@ -8498,13 +8498,13 @@
         <v>74.1157024793388</v>
       </c>
       <c r="M146" t="n">
-        <v>5.72505882352941</v>
+        <v>0.581577464788733</v>
       </c>
       <c r="N146" t="n">
-        <v>4.38388235294118</v>
+        <v>0.460943661971831</v>
       </c>
       <c r="O146" t="n">
-        <v>5.39529411764706</v>
+        <v>0.488633802816902</v>
       </c>
     </row>
     <row r="147">
@@ -8545,13 +8545,13 @@
         <v>95.2354570637119</v>
       </c>
       <c r="M147" t="n">
-        <v>5.4991131498471</v>
+        <v>0.529689243027889</v>
       </c>
       <c r="N147" t="n">
-        <v>4.11247706422018</v>
+        <v>0.429298804780877</v>
       </c>
       <c r="O147" t="n">
-        <v>5.4705504587156</v>
+        <v>0.480916334661355</v>
       </c>
     </row>
     <row r="148">
@@ -8592,13 +8592,13 @@
         <v>93.8888888888889</v>
       </c>
       <c r="M148" t="n">
-        <v>5.52921739130435</v>
+        <v>0.57051948051948</v>
       </c>
       <c r="N148" t="n">
-        <v>4.01704347826087</v>
+        <v>0.378376623376623</v>
       </c>
       <c r="O148" t="n">
-        <v>5.42295652173913</v>
+        <v>0.457714285714286</v>
       </c>
     </row>
     <row r="149">
@@ -8639,13 +8639,13 @@
         <v>78.8395061728395</v>
       </c>
       <c r="M149" t="n">
-        <v>5.96972602739726</v>
+        <v>0.629923076923077</v>
       </c>
       <c r="N149" t="n">
-        <v>3.90575342465753</v>
+        <v>0.377115384615384</v>
       </c>
       <c r="O149" t="n">
-        <v>5.61191780821918</v>
+        <v>0.505807692307693</v>
       </c>
     </row>
     <row r="150">
@@ -8686,13 +8686,13 @@
         <v>60.1803152633603</v>
       </c>
       <c r="M150" t="n">
-        <v>5.84175342465753</v>
+        <v>0.582852842809365</v>
       </c>
       <c r="N150" t="n">
-        <v>3.99901369863014</v>
+        <v>0.368307692307693</v>
       </c>
       <c r="O150" t="n">
-        <v>5.58805479452055</v>
+        <v>0.439404682274248</v>
       </c>
     </row>
     <row r="151">
@@ -8733,13 +8733,13 @@
         <v>74.3396226415094</v>
       </c>
       <c r="M151" t="n">
-        <v>5.826</v>
+        <v>0.571539936102236</v>
       </c>
       <c r="N151" t="n">
-        <v>4.16915</v>
+        <v>0.437977635782747</v>
       </c>
       <c r="O151" t="n">
-        <v>5.5437</v>
+        <v>0.493741214057507</v>
       </c>
     </row>
     <row r="152">
@@ -8780,13 +8780,13 @@
         <v>88.0657439446367</v>
       </c>
       <c r="M152" t="n">
-        <v>5.71463157894737</v>
+        <v>0.551429184549356</v>
       </c>
       <c r="N152" t="n">
-        <v>4.00301754385965</v>
+        <v>0.394163090128756</v>
       </c>
       <c r="O152" t="n">
-        <v>5.57705263157895</v>
+        <v>0.435832618025751</v>
       </c>
     </row>
     <row r="153">
@@ -8827,13 +8827,13 @@
         <v>73.7240075614367</v>
       </c>
       <c r="M153" t="n">
-        <v>5.58088235294118</v>
+        <v>0.5628</v>
       </c>
       <c r="N153" t="n">
-        <v>4.01123529411765</v>
+        <v>0.432253846153846</v>
       </c>
       <c r="O153" t="n">
-        <v>5.47476470588235</v>
+        <v>0.466638461538462</v>
       </c>
     </row>
     <row r="154">
@@ -8874,13 +8874,13 @@
         <v>38.1917628342719</v>
       </c>
       <c r="M154" t="n">
-        <v>5.95691891891892</v>
+        <v>0.632346437346439</v>
       </c>
       <c r="N154" t="n">
-        <v>4.06224324324324</v>
+        <v>0.430302211302211</v>
       </c>
       <c r="O154" t="n">
-        <v>5.671</v>
+        <v>0.522922604422606</v>
       </c>
     </row>
     <row r="155">
@@ -8921,13 +8921,13 @@
         <v>107.7792</v>
       </c>
       <c r="M155" t="n">
-        <v>5.82512195121951</v>
+        <v>0.5881</v>
       </c>
       <c r="N155" t="n">
-        <v>4.02865853658537</v>
+        <v>0.398405</v>
       </c>
       <c r="O155" t="n">
-        <v>5.59239837398374</v>
+        <v>0.43125</v>
       </c>
     </row>
     <row r="156">
@@ -8968,13 +8968,13 @@
         <v>51.3037095814323</v>
       </c>
       <c r="M156" t="n">
-        <v>5.76632135306554</v>
+        <v>0.563195187165775</v>
       </c>
       <c r="N156" t="n">
-        <v>4.10976744186047</v>
+        <v>0.428275401069518</v>
       </c>
       <c r="O156" t="n">
-        <v>5.59221987315011</v>
+        <v>0.47253743315508</v>
       </c>
     </row>
     <row r="157">
@@ -9015,13 +9015,13 @@
         <v>37.63671875</v>
       </c>
       <c r="M157" t="n">
-        <v>5.32677130044843</v>
+        <v>0.421326923076922</v>
       </c>
       <c r="N157" t="n">
-        <v>4.06139013452915</v>
+        <v>0.391990384615384</v>
       </c>
       <c r="O157" t="n">
-        <v>5.28493273542601</v>
+        <v>0.353086538461539</v>
       </c>
     </row>
     <row r="158">
@@ -9062,13 +9062,13 @@
         <v>69.2717311906501</v>
       </c>
       <c r="M158" t="n">
-        <v>5.58992592592593</v>
+        <v>0.57575</v>
       </c>
       <c r="N158" t="n">
-        <v>3.8402962962963</v>
+        <v>0.374472727272728</v>
       </c>
       <c r="O158" t="n">
-        <v>5.58433333333333</v>
+        <v>0.485754545454545</v>
       </c>
     </row>
     <row r="159">
@@ -9109,13 +9109,13 @@
         <v>42.9362765514369</v>
       </c>
       <c r="M159" t="n">
-        <v>5.73251824817518</v>
+        <v>0.549109589041096</v>
       </c>
       <c r="N159" t="n">
-        <v>4.0735401459854</v>
+        <v>0.437337899543379</v>
       </c>
       <c r="O159" t="n">
-        <v>5.59259124087591</v>
+        <v>0.458328767123287</v>
       </c>
     </row>
     <row r="160">
@@ -9156,13 +9156,13 @@
         <v>141.698347107438</v>
       </c>
       <c r="M160" t="n">
-        <v>5.95683257918552</v>
+        <v>0.616024390243902</v>
       </c>
       <c r="N160" t="n">
-        <v>3.97588235294118</v>
+        <v>0.411164634146341</v>
       </c>
       <c r="O160" t="n">
-        <v>5.80647058823529</v>
+        <v>0.486939024390244</v>
       </c>
     </row>
     <row r="161">
@@ -9203,13 +9203,13 @@
         <v>59.78</v>
       </c>
       <c r="M161" t="n">
-        <v>5.68675862068966</v>
+        <v>0.552690909090909</v>
       </c>
       <c r="N161" t="n">
-        <v>4.07331034482759</v>
+        <v>0.388590909090909</v>
       </c>
       <c r="O161" t="n">
-        <v>5.56503448275862</v>
+        <v>0.418509090909091</v>
       </c>
     </row>
     <row r="162">
@@ -9250,13 +9250,13 @@
         <v>60.823361082206</v>
       </c>
       <c r="M162" t="n">
-        <v>5.44929078014184</v>
+        <v>0.50655</v>
       </c>
       <c r="N162" t="n">
-        <v>4.18281323877069</v>
+        <v>0.444315625</v>
       </c>
       <c r="O162" t="n">
-        <v>5.27853427895981</v>
+        <v>0.429959375</v>
       </c>
     </row>
     <row r="163">
@@ -9297,13 +9297,13 @@
         <v>64.5507942789304</v>
       </c>
       <c r="M163" t="n">
-        <v>5.70823671497585</v>
+        <v>0.565603149606298</v>
       </c>
       <c r="N163" t="n">
-        <v>3.94114734299517</v>
+        <v>0.407274015748032</v>
       </c>
       <c r="O163" t="n">
-        <v>5.64010869565217</v>
+        <v>0.460625196850395</v>
       </c>
     </row>
     <row r="164">
@@ -9344,13 +9344,13 @@
         <v>67.2692307692308</v>
       </c>
       <c r="M164" t="n">
-        <v>5.73743935309973</v>
+        <v>0.569469424460432</v>
       </c>
       <c r="N164" t="n">
-        <v>4.00339622641509</v>
+        <v>0.399246402877698</v>
       </c>
       <c r="O164" t="n">
-        <v>5.62936657681941</v>
+        <v>0.464676258992807</v>
       </c>
     </row>
     <row r="165">
@@ -9391,13 +9391,13 @@
         <v>34.2208333333333</v>
       </c>
       <c r="M165" t="n">
-        <v>5.69553892215569</v>
+        <v>0.575793774319066</v>
       </c>
       <c r="N165" t="n">
-        <v>4.05889221556886</v>
+        <v>0.403143968871595</v>
       </c>
       <c r="O165" t="n">
-        <v>5.47086826347305</v>
+        <v>0.454595330739299</v>
       </c>
     </row>
     <row r="166">
@@ -9438,13 +9438,13 @@
         <v>42.5568</v>
       </c>
       <c r="M166" t="n">
-        <v>5.50372413793103</v>
+        <v>0.477818181818182</v>
       </c>
       <c r="N166" t="n">
-        <v>4.38103448275862</v>
+        <v>0.505171717171717</v>
       </c>
       <c r="O166" t="n">
-        <v>5.48213793103448</v>
+        <v>0.503212121212121</v>
       </c>
     </row>
     <row r="167">
@@ -9485,13 +9485,13 @@
         <v>76.0054012345679</v>
       </c>
       <c r="M167" t="n">
-        <v>5.69117647058824</v>
+        <v>0.522634020618557</v>
       </c>
       <c r="N167" t="n">
-        <v>4.2238431372549</v>
+        <v>0.486747422680413</v>
       </c>
       <c r="O167" t="n">
-        <v>5.47611764705882</v>
+        <v>0.474871134020618</v>
       </c>
     </row>
     <row r="168">
@@ -9532,13 +9532,13 @@
         <v>27.1487603305785</v>
       </c>
       <c r="M168" t="n">
-        <v>5.99090909090909</v>
+        <v>0.568192771084337</v>
       </c>
       <c r="N168" t="n">
-        <v>4.1079797979798</v>
+        <v>0.431975903614458</v>
       </c>
       <c r="O168" t="n">
-        <v>5.71151515151515</v>
+        <v>0.506674698795181</v>
       </c>
     </row>
     <row r="169">
@@ -9579,13 +9579,13 @@
         <v>65.9058725531029</v>
       </c>
       <c r="M169" t="n">
-        <v>5.75269349845201</v>
+        <v>0.593528925619835</v>
       </c>
       <c r="N169" t="n">
-        <v>4.21637770897833</v>
+        <v>0.454028925619835</v>
       </c>
       <c r="O169" t="n">
-        <v>5.67467492260062</v>
+        <v>0.501210743801653</v>
       </c>
     </row>
     <row r="170">
@@ -9626,13 +9626,13 @@
         <v>125.46875</v>
       </c>
       <c r="M170" t="n">
-        <v>5.51473469387755</v>
+        <v>0.507365979381443</v>
       </c>
       <c r="N170" t="n">
-        <v>4.17612244897959</v>
+        <v>0.413505154639176</v>
       </c>
       <c r="O170" t="n">
-        <v>5.36424489795918</v>
+        <v>0.417113402061856</v>
       </c>
     </row>
     <row r="171">
@@ -9673,13 +9673,13 @@
         <v>68.7135717031911</v>
       </c>
       <c r="M171" t="n">
-        <v>5.56752613240418</v>
+        <v>0.537655021834061</v>
       </c>
       <c r="N171" t="n">
-        <v>4.22195121951219</v>
+        <v>0.459576419213974</v>
       </c>
       <c r="O171" t="n">
-        <v>5.43923344947735</v>
+        <v>0.47428384279476</v>
       </c>
     </row>
     <row r="172">
@@ -9720,13 +9720,13 @@
         <v>91.43</v>
       </c>
       <c r="M172" t="n">
-        <v>5.64068493150685</v>
+        <v>0.564016393442623</v>
       </c>
       <c r="N172" t="n">
-        <v>4.00506849315069</v>
+        <v>0.385622950819672</v>
       </c>
       <c r="O172" t="n">
-        <v>5.66150684931507</v>
+        <v>0.473622950819672</v>
       </c>
     </row>
     <row r="173">
@@ -9767,13 +9767,13 @@
         <v>71.8217448105676</v>
       </c>
       <c r="M173" t="n">
-        <v>5.93558773424191</v>
+        <v>0.617104938271606</v>
       </c>
       <c r="N173" t="n">
-        <v>4.02645655877342</v>
+        <v>0.416724279835391</v>
       </c>
       <c r="O173" t="n">
-        <v>5.69596252129472</v>
+        <v>0.504938271604938</v>
       </c>
     </row>
     <row r="174">
@@ -9814,13 +9814,13 @@
         <v>94.08</v>
       </c>
       <c r="M174" t="n">
-        <v>5.61970982142857</v>
+        <v>0.58693946731235</v>
       </c>
       <c r="N174" t="n">
-        <v>4.00037946428571</v>
+        <v>0.413539951573851</v>
       </c>
       <c r="O174" t="n">
-        <v>5.38267857142857</v>
+        <v>0.461803874092009</v>
       </c>
     </row>
     <row r="175">
@@ -9861,13 +9861,13 @@
         <v>68.1012491781723</v>
       </c>
       <c r="M175" t="n">
-        <v>5.72505836575875</v>
+        <v>0.579985221674877</v>
       </c>
       <c r="N175" t="n">
-        <v>4.09081712062257</v>
+        <v>0.436009852216748</v>
       </c>
       <c r="O175" t="n">
-        <v>5.56653696498054</v>
+        <v>0.539571428571429</v>
       </c>
     </row>
     <row r="176">
@@ -9908,13 +9908,13 @@
         <v>68.673536794821</v>
       </c>
       <c r="M176" t="n">
-        <v>5.56722129783694</v>
+        <v>0.562462809917356</v>
       </c>
       <c r="N176" t="n">
-        <v>4.15236272878536</v>
+        <v>0.456669421487602</v>
       </c>
       <c r="O176" t="n">
-        <v>5.47201331114809</v>
+        <v>0.486080578512396</v>
       </c>
     </row>
     <row r="177">
@@ -9955,13 +9955,13 @@
         <v>89.0625</v>
       </c>
       <c r="M177" t="n">
-        <v>5.6674358974359</v>
+        <v>0.56067816091954</v>
       </c>
       <c r="N177" t="n">
-        <v>3.9865811965812</v>
+        <v>0.405609195402299</v>
       </c>
       <c r="O177" t="n">
-        <v>5.44444444444444</v>
+        <v>0.470252873563218</v>
       </c>
     </row>
     <row r="178">
@@ -10002,13 +10002,13 @@
         <v>54.6361111111111</v>
       </c>
       <c r="M178" t="n">
-        <v>5.72007633587786</v>
+        <v>0.56213058419244</v>
       </c>
       <c r="N178" t="n">
-        <v>4.21972010178117</v>
+        <v>0.412938144329897</v>
       </c>
       <c r="O178" t="n">
-        <v>5.62501272264631</v>
+        <v>0.475666666666666</v>
       </c>
     </row>
     <row r="179">
@@ -10049,13 +10049,13 @@
         <v>71.4120982986768</v>
       </c>
       <c r="M179" t="n">
-        <v>5.59665680473373</v>
+        <v>0.555852631578948</v>
       </c>
       <c r="N179" t="n">
-        <v>4.23073964497041</v>
+        <v>0.482428070175438</v>
       </c>
       <c r="O179" t="n">
-        <v>5.45822485207101</v>
+        <v>0.525045614035088</v>
       </c>
     </row>
     <row r="180">
@@ -10096,13 +10096,13 @@
         <v>48.2920472265538</v>
       </c>
       <c r="M180" t="n">
-        <v>5.655546875</v>
+        <v>0.577100746268656</v>
       </c>
       <c r="N180" t="n">
-        <v>4.19747395833333</v>
+        <v>0.46705223880597</v>
       </c>
       <c r="O180" t="n">
-        <v>5.65252604166667</v>
+        <v>0.535705223880597</v>
       </c>
     </row>
     <row r="181">
@@ -10143,13 +10143,13 @@
         <v>102.3984375</v>
       </c>
       <c r="M181" t="n">
-        <v>5.45072289156627</v>
+        <v>0.514106382978724</v>
       </c>
       <c r="N181" t="n">
-        <v>4.0425702811245</v>
+        <v>0.448744680851064</v>
       </c>
       <c r="O181" t="n">
-        <v>5.46510040160643</v>
+        <v>0.455063829787234</v>
       </c>
     </row>
     <row r="182">
@@ -10190,13 +10190,13 @@
         <v>108.598337950139</v>
       </c>
       <c r="M182" t="n">
-        <v>5.71621951219512</v>
+        <v>0.574</v>
       </c>
       <c r="N182" t="n">
-        <v>4.20786585365854</v>
+        <v>0.479731884057971</v>
       </c>
       <c r="O182" t="n">
-        <v>5.63128048780488</v>
+        <v>0.52795652173913</v>
       </c>
     </row>
     <row r="183">
@@ -10237,13 +10237,13 @@
         <v>99.53125</v>
       </c>
       <c r="M183" t="n">
-        <v>5.44850746268657</v>
+        <v>0.50875</v>
       </c>
       <c r="N183" t="n">
-        <v>4.2355223880597</v>
+        <v>0.474604166666667</v>
       </c>
       <c r="O183" t="n">
-        <v>5.43791044776119</v>
+        <v>0.510333333333333</v>
       </c>
     </row>
     <row r="184">
@@ -10284,13 +10284,13 @@
         <v>63.1834319526627</v>
       </c>
       <c r="M184" t="n">
-        <v>5.64236559139785</v>
+        <v>0.552506172839506</v>
       </c>
       <c r="N184" t="n">
-        <v>4.16666666666667</v>
+        <v>0.44958024691358</v>
       </c>
       <c r="O184" t="n">
-        <v>5.53236559139785</v>
+        <v>0.466246913580247</v>
       </c>
     </row>
     <row r="185">
@@ -10331,13 +10331,13 @@
         <v>69.609375</v>
       </c>
       <c r="M185" t="n">
-        <v>5.52771929824561</v>
+        <v>0.56664705882353</v>
       </c>
       <c r="N185" t="n">
-        <v>4.14438596491228</v>
+        <v>0.431382352941176</v>
       </c>
       <c r="O185" t="n">
-        <v>5.48035087719298</v>
+        <v>0.493764705882353</v>
       </c>
     </row>
     <row r="186">
@@ -10378,13 +10378,13 @@
         <v>98.328125</v>
       </c>
       <c r="M186" t="n">
-        <v>5.86725806451613</v>
+        <v>0.630302325581395</v>
       </c>
       <c r="N186" t="n">
-        <v>4.24193548387097</v>
+        <v>0.477279069767442</v>
       </c>
       <c r="O186" t="n">
-        <v>5.6441935483871</v>
+        <v>0.487558139534884</v>
       </c>
     </row>
     <row r="187">
@@ -10425,13 +10425,13 @@
         <v>75.8061224489796</v>
       </c>
       <c r="M187" t="n">
-        <v>5.71021582733813</v>
+        <v>0.56447</v>
       </c>
       <c r="N187" t="n">
-        <v>4.08726618705036</v>
+        <v>0.42699</v>
       </c>
       <c r="O187" t="n">
-        <v>5.52474820143885</v>
+        <v>0.47802</v>
       </c>
     </row>
     <row r="188">
@@ -10472,13 +10472,13 @@
         <v>65.92</v>
       </c>
       <c r="M188" t="n">
-        <v>5.52035714285714</v>
+        <v>0.553741935483871</v>
       </c>
       <c r="N188" t="n">
-        <v>3.9375</v>
+        <v>0.43341935483871</v>
       </c>
       <c r="O188" t="n">
-        <v>5.43130952380952</v>
+        <v>0.457951612903226</v>
       </c>
     </row>
     <row r="189">
@@ -10519,13 +10519,13 @@
         <v>87.72</v>
       </c>
       <c r="M189" t="n">
-        <v>6.31078947368421</v>
+        <v>0.633457142857143</v>
       </c>
       <c r="N189" t="n">
-        <v>3.76289473684211</v>
+        <v>0.386542857142857</v>
       </c>
       <c r="O189" t="n">
-        <v>5.82368421052632</v>
+        <v>0.4734</v>
       </c>
     </row>
     <row r="190">
@@ -10566,13 +10566,13 @@
         <v>66.1111111111111</v>
       </c>
       <c r="M190" t="n">
-        <v>5.76545454545455</v>
+        <v>0.625428571428571</v>
       </c>
       <c r="N190" t="n">
-        <v>4.02779220779221</v>
+        <v>0.437892857142857</v>
       </c>
       <c r="O190" t="n">
-        <v>5.53</v>
+        <v>0.556964285714286</v>
       </c>
     </row>
     <row r="191">
@@ -10613,13 +10613,13 @@
         <v>118.691358024691</v>
       </c>
       <c r="M191" t="n">
-        <v>6.14258064516129</v>
+        <v>0.692180555555555</v>
       </c>
       <c r="N191" t="n">
-        <v>4.1952688172043</v>
+        <v>0.399486111111111</v>
       </c>
       <c r="O191" t="n">
-        <v>5.8594623655914</v>
+        <v>0.548347222222222</v>
       </c>
     </row>
     <row r="192">
@@ -10660,13 +10660,13 @@
         <v>88.14</v>
       </c>
       <c r="M192" t="n">
-        <v>5.73521126760563</v>
+        <v>0.589541984732824</v>
       </c>
       <c r="N192" t="n">
-        <v>3.94140845070423</v>
+        <v>0.431931297709924</v>
       </c>
       <c r="O192" t="n">
-        <v>5.68323943661972</v>
+        <v>0.484488549618321</v>
       </c>
     </row>
     <row r="193">
@@ -10707,13 +10707,13 @@
         <v>75.4567901234568</v>
       </c>
       <c r="M193" t="n">
-        <v>5.55764705882353</v>
+        <v>0.566162790697675</v>
       </c>
       <c r="N193" t="n">
-        <v>4.22168067226891</v>
+        <v>0.473848837209303</v>
       </c>
       <c r="O193" t="n">
-        <v>5.6118487394958</v>
+        <v>0.506895348837209</v>
       </c>
     </row>
     <row r="194">
@@ -10754,13 +10754,13 @@
         <v>44.6342975206612</v>
       </c>
       <c r="M194" t="n">
-        <v>5.64436224489796</v>
+        <v>0.555429032258065</v>
       </c>
       <c r="N194" t="n">
-        <v>4.05854591836735</v>
+        <v>0.43796129032258</v>
       </c>
       <c r="O194" t="n">
-        <v>5.42859693877551</v>
+        <v>0.48636129032258</v>
       </c>
     </row>
     <row r="195">
@@ -10801,13 +10801,13 @@
         <v>52.9583333333333</v>
       </c>
       <c r="M195" t="n">
-        <v>5.64715909090909</v>
+        <v>0.543405405405405</v>
       </c>
       <c r="N195" t="n">
-        <v>4.18113636363636</v>
+        <v>0.436</v>
       </c>
       <c r="O195" t="n">
-        <v>5.57965909090909</v>
+        <v>0.493351351351352</v>
       </c>
     </row>
     <row r="196">
@@ -10848,13 +10848,13 @@
         <v>33.8488888888889</v>
       </c>
       <c r="M196" t="n">
-        <v>5.74345679012346</v>
+        <v>0.557865384615384</v>
       </c>
       <c r="N196" t="n">
-        <v>3.92555555555556</v>
+        <v>0.419865384615385</v>
       </c>
       <c r="O196" t="n">
-        <v>5.50938271604938</v>
+        <v>0.491769230769231</v>
       </c>
     </row>
     <row r="197">
@@ -10895,13 +10895,13 @@
         <v>96.1833910034602</v>
       </c>
       <c r="M197" t="n">
-        <v>5.4683904109589</v>
+        <v>0.509436440677967</v>
       </c>
       <c r="N197" t="n">
-        <v>4.17869863013699</v>
+        <v>0.497512711864407</v>
       </c>
       <c r="O197" t="n">
-        <v>5.3947602739726</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="198">
@@ -10942,13 +10942,13 @@
         <v>97.3298647242456</v>
       </c>
       <c r="M198" t="n">
-        <v>5.74576388888889</v>
+        <v>0.579981818181818</v>
       </c>
       <c r="N198" t="n">
-        <v>3.98298611111111</v>
+        <v>0.400640909090909</v>
       </c>
       <c r="O198" t="n">
-        <v>5.55347222222222</v>
+        <v>0.486372727272727</v>
       </c>
     </row>
     <row r="199">
@@ -10989,13 +10989,13 @@
         <v>42.3575510204082</v>
       </c>
       <c r="M199" t="n">
-        <v>5.86381642512077</v>
+        <v>0.615841530054645</v>
       </c>
       <c r="N199" t="n">
-        <v>4.21652173913044</v>
+        <v>0.451672131147541</v>
       </c>
       <c r="O199" t="n">
-        <v>5.59666666666667</v>
+        <v>0.519825136612022</v>
       </c>
     </row>
     <row r="200">
@@ -11036,13 +11036,13 @@
         <v>45.0986121256391</v>
       </c>
       <c r="M200" t="n">
-        <v>5.34227053140097</v>
+        <v>0.525734567901235</v>
       </c>
       <c r="N200" t="n">
-        <v>4.17304347826087</v>
+        <v>0.473895061728395</v>
       </c>
       <c r="O200" t="n">
-        <v>5.42647342995169</v>
+        <v>0.49558024691358</v>
       </c>
     </row>
     <row r="201">
@@ -11065,7 +11065,7 @@
         <v>17</v>
       </c>
       <c r="G201" t="n">
-        <v>6.31674031751571</v>
+        <v>6.3167403175157</v>
       </c>
       <c r="H201" t="n">
         <v>0.727142857142857</v>
@@ -11083,13 +11083,13 @@
         <v>48.9328125</v>
       </c>
       <c r="M201" t="n">
-        <v>5.67037974683544</v>
+        <v>0.559680965147453</v>
       </c>
       <c r="N201" t="n">
-        <v>3.99601265822785</v>
+        <v>0.417890080428955</v>
       </c>
       <c r="O201" t="n">
-        <v>5.53333333333333</v>
+        <v>0.485525469168901</v>
       </c>
     </row>
     <row r="202">
@@ -11130,13 +11130,13 @@
         <v>82.434375</v>
       </c>
       <c r="M202" t="n">
-        <v>5.65599423631124</v>
+        <v>0.595516</v>
       </c>
       <c r="N202" t="n">
-        <v>4.01158501440922</v>
+        <v>0.427952</v>
       </c>
       <c r="O202" t="n">
-        <v>5.60922190201729</v>
+        <v>0.4965</v>
       </c>
     </row>
     <row r="203">
@@ -11177,13 +11177,13 @@
         <v>46.5712198685172</v>
       </c>
       <c r="M203" t="n">
-        <v>5.6426582278481</v>
+        <v>0.557990384615384</v>
       </c>
       <c r="N203" t="n">
-        <v>4.07679324894515</v>
+        <v>0.444096153846154</v>
       </c>
       <c r="O203" t="n">
-        <v>5.62966244725738</v>
+        <v>0.499879807692309</v>
       </c>
     </row>
     <row r="204">
@@ -11224,13 +11224,13 @@
         <v>35.2825484764543</v>
       </c>
       <c r="M204" t="n">
-        <v>5.58223300970874</v>
+        <v>0.555341176470589</v>
       </c>
       <c r="N204" t="n">
-        <v>4.05300970873786</v>
+        <v>0.442141176470588</v>
       </c>
       <c r="O204" t="n">
-        <v>5.52077669902913</v>
+        <v>0.472905882352941</v>
       </c>
     </row>
     <row r="205">
@@ -11271,13 +11271,13 @@
         <v>52.3408947700063</v>
       </c>
       <c r="M205" t="n">
-        <v>5.96148325358852</v>
+        <v>0.589866666666667</v>
       </c>
       <c r="N205" t="n">
-        <v>4.00258373205742</v>
+        <v>0.443350617283951</v>
       </c>
       <c r="O205" t="n">
-        <v>5.60210526315789</v>
+        <v>0.46476049382716</v>
       </c>
     </row>
     <row r="206">
@@ -11318,13 +11318,13 @@
         <v>51.2875</v>
       </c>
       <c r="M206" t="n">
-        <v>5.60828571428571</v>
+        <v>0.577269230769231</v>
       </c>
       <c r="N206" t="n">
-        <v>4.10428571428571</v>
+        <v>0.453192307692307</v>
       </c>
       <c r="O206" t="n">
-        <v>5.53442857142857</v>
+        <v>0.526519230769231</v>
       </c>
     </row>
     <row r="207">
@@ -11365,13 +11365,13 @@
         <v>34.3163265306122</v>
       </c>
       <c r="M207" t="n">
-        <v>5.9701724137931</v>
+        <v>0.550871794871795</v>
       </c>
       <c r="N207" t="n">
-        <v>4.16034482758621</v>
+        <v>0.411871794871795</v>
       </c>
       <c r="O207" t="n">
-        <v>5.84965517241379</v>
+        <v>0.467435897435897</v>
       </c>
     </row>
     <row r="208">
@@ -11412,13 +11412,13 @@
         <v>47.5280276816609</v>
       </c>
       <c r="M208" t="n">
-        <v>5.55182341650672</v>
+        <v>0.549316628701595</v>
       </c>
       <c r="N208" t="n">
-        <v>4.19760076775432</v>
+        <v>0.44696583143508</v>
       </c>
       <c r="O208" t="n">
-        <v>5.48305182341651</v>
+        <v>0.491132118451025</v>
       </c>
     </row>
     <row r="209">
@@ -11459,13 +11459,13 @@
         <v>64.1144996347699</v>
       </c>
       <c r="M209" t="n">
-        <v>5.67678431372549</v>
+        <v>0.561813299232736</v>
       </c>
       <c r="N209" t="n">
-        <v>4.19039215686275</v>
+        <v>0.445659846547315</v>
       </c>
       <c r="O209" t="n">
-        <v>5.65074509803922</v>
+        <v>0.503225063938619</v>
       </c>
     </row>
     <row r="210">
@@ -11506,13 +11506,13 @@
         <v>63.2592592592593</v>
       </c>
       <c r="M210" t="n">
-        <v>5.66191176470588</v>
+        <v>0.55405</v>
       </c>
       <c r="N210" t="n">
-        <v>3.87382352941176</v>
+        <v>0.3765</v>
       </c>
       <c r="O210" t="n">
-        <v>5.58426470588235</v>
+        <v>0.46535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>